<commit_message>
Fixed keyhandling issue in automation
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7242" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7403" uniqueCount="173">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -122,169 +122,13 @@
     <t>SettingsButtonDisabled</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_isIconDisplayed=QuitButton_xpath,true
-validate_isIconDisplayed=MinimizeButton_xpath,true
-validate_isIconDisplayed=ReloadButton_xpath,true
-validate_isIconDisplayed=ForwardButton_xpath,true
-validate_isIconDisplayed=BackButton_xpath,true
-validate_isIconDisplayed=GoButton_xpath,true
-validate_isIconDisplayed=HomeButton_xpath,true
-validate_isIconDisplayed=Addressbar_xpath,true
-validate_isIconDisplayed=SipButton_xpath,true
-validate_isIconDisplayed=ZoomtextButton_xpath,true
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_isIconDisplayed=QuitButton_xpath,false
-validate_isIconDisplayed=MinimizeButton_xpath,false
-validate_isIconDisplayed=ReloadButton_xpath,false
-validate_isIconDisplayed=ForwardButton_xpath,false
-validate_isIconDisplayed=BackButton_xpath,false
-validate_isIconDisplayed=GoButton_xpath,false
-validate_isIconDisplayed=HomeButton_xpath,false
-validate_isIconDisplayed=Addressbar_xpath,false
-validate_isIconDisplayed=SipButton_xpath,false
-validate_isIconDisplayed=ZoomtextButton_xpath,false
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-004
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-005
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-006
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-007
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-008
-};</t>
-  </si>
-  <si>
     <t>PageZoomEnabled as 4.0</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-009
-};</t>
   </si>
   <si>
     <t>PageZoomEnabled as -1.0</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-010
-};</t>
-  </si>
-  <si>
     <t xml:space="preserve">FullScreenDisabled </t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-011
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-012
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(8);
-validate1;
-TakeScreenshot(VT187-013);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/SplashScreen,SplashScreenPath,&lt;SplashScreenPath value="file://%INSTALLDIR%/images/moto.png"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-013
-};</t>
-  </si>
-  <si>
-    <t>wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://www.google.com" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>wait(4);
@@ -293,76 +137,6 @@
 wait(4);
 PullConfigxml;
 ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-006);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="2.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-007);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="3.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-009);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="-1.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-008);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="4.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-010);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="SignatureCapture~left:30semicolontop:130semicolonheight:100semicolonbgcolor:#663300semicolonwidth:200semicolonborder:visiblesemicolonvisibility:visible"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-011);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Signal~left:20semicolontop:300semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-012);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Battery~left:10semicolontop:200semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
 PushConfigxml;</t>
   </si>
   <si>
@@ -375,78 +149,11 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-TakeScreenshot(VT187-004);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-TakeScreenshot(VT187-005);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="1.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_Screenshot=VT187-014
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(2);
-TakeScreenshot(VT187-014);
-validate1;
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Google
 };
 </t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_isIconDisplayed=SettingsButton_xpath,true
-}</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-EnterData(Pwdenter_xpath,1234);
-ClickNativeIcon(PwdOK_xpath);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>wait(6);
@@ -457,16 +164,6 @@
 ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
 ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="0"/&gt;);
 PushConfigxml;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};
-validate2
-{
-validate_isIconDisplayed=SettingsButton_xpath,false
-};</t>
   </si>
   <si>
     <t>SettingsButtonProtection password</t>
@@ -520,12 +217,6 @@
 </t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Google
-};</t>
-  </si>
-  <si>
     <t xml:space="preserve">wait(6);
 validate1;
 SwitchApp(NATIVE_APP);
@@ -540,22 +231,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-EnterData(Pwdenter_xpath,4321);
-ClickNativeIcon(PwdOK_xpath);
-CheckUITextContains(Invalid_Password);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;)
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t>Exit Password  Without enterPwd</t>
   </si>
   <si>
@@ -563,20 +238,6 @@
   </si>
   <si>
     <t>Exit Password Enabled with Pwd exceeds</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-EnterData(Pwdenter_xpath,12345678910112233333454455666755555);
-ClickNativeIcon(PwdOK_xpath);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>SettingsButtonProtection password Exceeds</t>
@@ -699,26 +360,6 @@
     <t>SIP Debug Button</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-029
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-030
-};</t>
-  </si>
-  <si>
     <t>Zoom Debug Button(ClickTwice)</t>
   </si>
   <si>
@@ -738,34 +379,6 @@
 ClickNativeIcon(BackButton_xpath);
 ClickNativeIcon(ForwardButton_xpath);
 SwitchApp(WEBVIEW);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SipButton_xpath);
-TakeScreenshot(VT187-029);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(ZoomtextButton_xpath);
-ClickNativeIcon(ZoomtextButton_xpath);
-TakeScreenshot(VT187-030);
 validate2;
 wait(4);
 PullConfigxml;
@@ -804,9 +417,6 @@
 PullConfigxml;
 ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="0"/&gt;);
 PushConfigxml;</t>
-  </si>
-  <si>
-    <t>Navigation Timeout</t>
   </si>
   <si>
     <t>wait(6);
@@ -891,6 +501,447 @@
 PushConfigxml;</t>
   </si>
   <si>
+    <t>ServerCookie Validation</t>
+  </si>
+  <si>
+    <t>Exit Password  Press Cancel</t>
+  </si>
+  <si>
+    <t>wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+EnterData(ExitPwdenter_xpath,1234);
+ClickNativeIcon(PwdOK_xpath);
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+EnterData(ExitPwdenter_xpath,12345678910112233333454455666755555);
+ClickNativeIcon(PwdOK_xpath);
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+EnterData(ExitPwdenter_xpath,4321);
+ClickNativeIcon(PwdOK_xpath);
+CheckUITextContains(Invalid_Password);
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;)
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_isIconDisplayed=QuitButton_xpath,true
+validate_isIconDisplayed=MinimizeButton_xpath,true
+validate_isIconDisplayed=ReloadButton_xpath,true
+validate_isIconDisplayed=ForwardButton_xpath,true
+validate_isIconDisplayed=BackButton_xpath,true
+validate_isIconDisplayed=GoButton_xpath,true
+validate_isIconDisplayed=HomeButton_xpath,true
+validate_isIconDisplayed=Addressbar_xpath,true
+validate_isIconDisplayed=SipButton_xpath,true
+validate_isIconDisplayed=ZoomtextButton_xpath,true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_isIconDisplayed=QuitButton_xpath,false
+validate_isIconDisplayed=MinimizeButton_xpath,false
+validate_isIconDisplayed=ReloadButton_xpath,false
+validate_isIconDisplayed=ForwardButton_xpath,false
+validate_isIconDisplayed=BackButton_xpath,false
+validate_isIconDisplayed=GoButton_xpath,false
+validate_isIconDisplayed=HomeButton_xpath,false
+validate_isIconDisplayed=Addressbar_xpath,false
+validate_isIconDisplayed=SipButton_xpath,false
+validate_isIconDisplayed=ZoomtextButton_xpath,false
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-004
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-005
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-006
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-007
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-008
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-009
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-010
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-011
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-012
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-013
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=All Index
+};
+validate1
+{
+validate_PageTitle=All Index
+};
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_isIconDisplayed=SettingsButton_xpath,true
+}</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_isIconDisplayed=SettingsButton_xpath,false
+};</t>
+  </si>
+  <si>
+    <t>SettingsButton Protection Password  Press Cancel</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=All Index
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+ClickNativeIcon(SettingPwd_cancel_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+ClickNativeIcon(ExitPwd_cancel_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+TakeScreenshot(VT187-001);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-001
+};</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+TakeScreenshot(VT187-002);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="1.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-002
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-003);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="2.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-003
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-004);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="3.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-005);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="4.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-006);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="-1.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-007);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="SignatureCapture~left:30semicolontop:130semicolonheight:100semicolonbgcolor:#663300semicolonwidth:200semicolonborder:visiblesemicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-008);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Signal~left:20semicolontop:300semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-009);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Battery~left:10semicolontop:200semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(8);
+validate1;
+TakeScreenshot(VT187-010);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/SplashScreen,SplashScreenPath,&lt;SplashScreenPath value="file://%INSTALLDIR%/images/moto.png"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(2);
+TakeScreenshot(VT187-011);
+validate1;
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SipButton_xpath);
+TakeScreenshot(VT187-012);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(ZoomtextButton_xpath);
+ClickNativeIcon(ZoomtextButton_xpath);
+TakeScreenshot(VT187-013);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
     <t>wait(6);
 validate1;
 wait(4);
@@ -899,7 +950,495 @@
 validate2;
 wait(4);
 PullConfigxml;
-ChangeConfigxml(Configuration/DeviceKeys,FunctionKeysCapturable, &lt;FunctionKeysCapturable   value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9097/1_Browser_Validation/cookie/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>Default Navigation Timeout value</t>
+  </si>
+  <si>
+    <t>User defined Navigation Timeout value</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="30000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>Default Navigation Timeout badlink file</t>
+  </si>
+  <si>
+    <t>User defined Navigation Timeout badlink file</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/abcd.html"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>Invalid Navigation Timeout value</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(32);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="-100"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>Invalid Navigation Timeout badlink file</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/menu.html"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Index of /1_Browser_Validation/cookie
+};
+validate2
+{
+validate_Page=CookieCreation_xpath,This
+}</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(ServerCookie_test_link);
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://10.233.85.82:9097/1_Browser_Validation/cookie/servercookie.php?set=yes);
+ClickNativeIcon(GoButton_xpath);
+ClickNativeIcon(GoButton_xpath);
+ClickNativeIcon(ReloadButton_xpath);
+SwitchApp(WEBVIEW);
+wait(4);
+validate2;
+wait(4);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2679 - check the message box after resume the device with HostURL set  other device ip address in config with default Timeoutvalue</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="http://www.google.com"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Connecting to Google.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=badlinkpage
+};
+validate3
+{
+validate_PageTitle=BadLink
+};</t>
+  </si>
+  <si>
+    <t>VT187-2676 - check the message box after resume the device with HostURL set in config with default Timeoutvalue</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Connecting_to_Google..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9095"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2680 - check the message box after resume the device with HostURL set  other device ip address with port set to 9097 in config with default Timeoutvalue</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9097"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="wait till connection successfull"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2681 - check the message box after resume the device with HostURL set  other device ip address with port set to 9095 in config with default Timeoutvalue</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(wait_till_connection_successfull);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="127.0.0.1"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2682 - check the message box after resume the device with HostURL set  other device ip address in config with default Timeoutvalue</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="111.222.11.00"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2683 - check the message box after resume the device with HostURL set  ip address which does not exists in config with default Timeoutvalue</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(25);
+validate3;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="60000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2685 - check the message box after resume the device with message set and  Timeoutvalue set to 60 seconds</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate2;
+wait(40);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="15000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2686 - check the message box after resume the device with message set and   Timeoutvalue set to 15 seconds</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="5000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2687 - check the message box after resume the device with message set and   Timeoutvalue set to 5 seconds</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2688 - check the message box after resume the device with message set and   Timeoutvalue set to 0 seconds</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="-15000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2689 - check the message box after resume the device with Timeoutvalue set to -15  seconds</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout, );
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2684 - check the message box after resume the device without Timeoutvalue tag default value</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(back);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-2697 - message box on minimize and restore application</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(back);
+CheckUITextContains(Establishing_Connection..);
+press_Key(Home);
+wait(1);
+validate2;
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wifi_Mode(on);
+press_Key(back);
+wait(5);
+CheckUITextContains(voidConnection);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection,&lt;TrackConnection value="0" /&gt;);
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_AppMinimized=homescreen
+};
+validate3
+{
+validate_PageTitle=All Index
+};</t>
+  </si>
+  <si>
+    <t>VT187-0660 - Preload with NPAPI plugin PreloadLegacyGeneric</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=PB and RE2.2 Semi Auto Frame Work : SignatureCapture
+};
+validate2
+{
+validate_isIconDisplayed=signatureArea_xpath,true
+};</t>
+  </si>
+  <si>
+    <t>VT187-0661 - Do not Preload with NPAPI plugin PreloadLegacyGeneric</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=PB and RE2.2 Semi Auto Frame Work : SignatureCapture
+};
+validate2
+{
+validate_isIconDisplayed=signatureArea_xpath,false
+};</t>
+  </si>
+  <si>
+    <t>VT187-0670 - Preload with NPAPI plugin PreloadJSObjects</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VT187-0671 - Do not Preload with NPAPI plugin PreloadJSObjects</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
 PushConfigxml;</t>
   </si>
 </sst>
@@ -955,7 +1494,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1051,22 +1590,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1098,7 +1626,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1395,9 +1929,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD41"/>
+  <dimension ref="A1:XFD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1405,9 +1939,9 @@
     <col min="2" max="2" width="7.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="6.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="6.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="44.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="88.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="51.85546875" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
@@ -1469,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -1485,7 +2019,9 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1496,10 +2032,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1512,7 +2048,9 @@
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1523,10 +2061,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
@@ -39074,21 +39612,23 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -39101,7 +39641,9 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
@@ -39112,10 +39654,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -39128,7 +39670,9 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
@@ -39139,10 +39683,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -39155,7 +39699,9 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
@@ -39166,10 +39712,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -39182,7 +39728,9 @@
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
@@ -39193,10 +39741,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -39209,21 +39757,23 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -39236,21 +39786,23 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39263,7 +39815,9 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
@@ -39274,10 +39828,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -39290,7 +39844,9 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
@@ -39301,10 +39857,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>44</v>
+        <v>92</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -39317,7 +39873,9 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>10</v>
       </c>
@@ -39328,10 +39886,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -39344,7 +39902,9 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
       </c>
@@ -39355,10 +39915,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39371,7 +39931,9 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
@@ -39382,10 +39944,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39398,21 +39960,23 @@
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -39425,7 +39989,9 @@
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
@@ -39436,10 +40002,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -39452,129 +40018,139 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="128.25" thickBot="1">
+    <row r="20" spans="1:11" ht="192" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="166.5" thickBot="1">
+    <row r="21" spans="1:11" ht="128.25" thickBot="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="230.25" thickBot="1">
+    <row r="22" spans="1:11" ht="166.5" thickBot="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="243" thickBot="1">
+    <row r="23" spans="1:11" ht="230.25" thickBot="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -39587,129 +40163,139 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="179.25" thickBot="1">
+    <row r="25" spans="1:11" ht="243" thickBot="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="166.5" thickBot="1">
+    <row r="26" spans="1:11" ht="179.25" thickBot="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="204.75" thickBot="1">
+    <row r="27" spans="1:11" ht="192" thickBot="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="179.25" thickBot="1">
+    <row r="28" spans="1:11" ht="166.5" thickBot="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -39722,21 +40308,23 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -39749,102 +40337,110 @@
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="192" thickBot="1">
+    <row r="31" spans="1:11" ht="204.75" thickBot="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="128.25" thickBot="1">
+    <row r="32" spans="1:11" ht="179.25" thickBot="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="102.75" thickBot="1">
+    <row r="33" spans="1:11" ht="192" thickBot="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -39857,102 +40453,110 @@
       <c r="B34" s="1">
         <v>1</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="128.25" thickBot="1">
+    <row r="35" spans="1:11" ht="102.75" thickBot="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>109</v>
+        <v>69</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="141" thickBot="1">
+    <row r="36" spans="1:11" ht="128.25" thickBot="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="128.25" thickBot="1">
+    <row r="37" spans="1:11" ht="141" thickBot="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -39965,64 +40569,731 @@
       <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+    <row r="39" spans="1:11" ht="141" thickBot="1">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+    <row r="40" spans="1:11" ht="166.5" thickBot="1">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
+    <row r="41" spans="1:11" ht="166.5" thickBot="1">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" ht="141" thickBot="1">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" ht="166.5" thickBot="1">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" ht="268.5" thickBot="1">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" ht="204.75" thickBot="1">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11" ht="204.75" thickBot="1">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11" ht="204.75" thickBot="1">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="1">
+        <v>1</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" ht="204.75" thickBot="1">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" ht="166.5" thickBot="1">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" ht="243" thickBot="1">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+    </row>
+    <row r="57" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="204.75" thickBot="1">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="268.5" thickBot="1">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="11">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="115.5" thickBot="1">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="11">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed network issues in DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7403" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7403" uniqueCount="175">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -131,24 +131,6 @@
     <t xml:space="preserve">FullScreenDisabled </t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Google
@@ -156,79 +138,10 @@
 </t>
   </si>
   <si>
-    <t>wait(6);
-validate1;
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="0"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>SettingsButtonProtection password</t>
   </si>
   <si>
     <t>SettingsButtonProtection Invalid password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-EnterData(SettingPwdenter_xpath,1234);
-ClickNativeIcon(SettingsPwdOK_xpath);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-EnterData(SettingPwdenter_xpath,4321);
-ClickNativeIcon(SettingsPwdOK_xpath);
-CheckUITextContains(password_wrong);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-ClickNativeIcon(PwdOK_xpath);
-CheckUITextContains(Invalid_Password);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-PushConfigxml;
-</t>
   </si>
   <si>
     <t>Exit Password  Without enterPwd</t>
@@ -243,38 +156,7 @@
     <t>SettingsButtonProtection password Exceeds</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-EnterData(SettingPwdenter_xpath,12345678910112233445566666);
-ClickNativeIcon(SettingsPwdOK_xpath);
-CheckUITextContains(password_wrong);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t>Home Debug Button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-ClickNativeIcon(SettingsPwdOK_xpath);
-CheckUITextContains(password_wrong);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
   </si>
   <si>
     <t xml:space="preserve">validate1
@@ -287,36 +169,7 @@
     <t>Go Debug Button</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-link_Click(PBAndroid_test_link);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(HomeButton_xpath);
-validate1;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Back Debug Button </t>
-  </si>
-  <si>
-    <t>wait(6);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-TypeinAddressbar(Addressbar_xpath,http://www.google.com);
-ClickNativeIcon(GoButton_xpath);
-SwitchApp(WEBVIEW);
-wait(8);
-validate1;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>validate1
@@ -330,20 +183,6 @@
   </si>
   <si>
     <t>Forward Debug Button</t>
-  </si>
-  <si>
-    <t>wait(4);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(BackButton_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t xml:space="preserve">validate1
@@ -372,62 +211,13 @@
 };</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(BackButton_xpath);
-ClickNativeIcon(ForwardButton_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t>Void Connection Enabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(MinimizeButton_xpath);
-validate_AppMinimized(appsscreen);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
-PushConfigxml;
-</t>
   </si>
   <si>
     <t>Void Connection Timeout</t>
   </si>
   <si>
     <t>Void Connection Disbaled</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-wait(4);
-CheckUITextContains(Establishing_Connection...);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="0"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-wait(4);
-CheckUITextContains(voidConnection);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>validate1
@@ -507,57 +297,6 @@
     <t>Exit Password  Press Cancel</t>
   </si>
   <si>
-    <t>wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-EnterData(ExitPwdenter_xpath,1234);
-ClickNativeIcon(PwdOK_xpath);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-EnterData(ExitPwdenter_xpath,12345678910112233333454455666755555);
-ClickNativeIcon(PwdOK_xpath);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-EnterData(ExitPwdenter_xpath,4321);
-ClickNativeIcon(PwdOK_xpath);
-CheckUITextContains(Invalid_Password);
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;)
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=All Index
@@ -632,56 +371,6 @@
 };
 validate2
 {
-validate_Screenshot=VT187-007
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-008
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-009
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-010
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-011
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
 validate_Screenshot=VT187-012
 };</t>
   </si>
@@ -693,37 +382,6 @@
 validate2
 {
 validate_Screenshot=VT187-013
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=All Index
-};
-validate1
-{
-validate_PageTitle=All Index
-};
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_isIconDisplayed=SettingsButton_xpath,true
-}</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_isIconDisplayed=SettingsButton_xpath,false
 };</t>
   </si>
   <si>
@@ -740,86 +398,6 @@
 };</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-ClickNativeIcon(SettingPwd_cancel_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-ClickNativeIcon(ExitPwd_cancel_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-TakeScreenshot(VT187-001);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-001
-};</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-TakeScreenshot(VT187-002);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="1.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-002
-};</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-003);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="2.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=All Index
@@ -828,118 +406,6 @@
 {
 validate_Screenshot=VT187-003
 };</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-004);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="3.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-005);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="4.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-006);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="-1.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-007);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="SignatureCapture~left:30semicolontop:130semicolonheight:100semicolonbgcolor:#663300semicolonwidth:200semicolonborder:visiblesemicolonvisibility:visible"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-008);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Signal~left:20semicolontop:300semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-009);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Battery~left:10semicolontop:200semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(8);
-validate1;
-TakeScreenshot(VT187-010);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/SplashScreen,SplashScreenPath,&lt;SplashScreenPath value="file://%INSTALLDIR%/images/moto.png"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(2);
-TakeScreenshot(VT187-011);
-validate1;
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SipButton_xpath);
-TakeScreenshot(VT187-012);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(ZoomtextButton_xpath);
-ClickNativeIcon(ZoomtextButton_xpath);
-TakeScreenshot(VT187-013);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
   </si>
   <si>
     <t>wait(6);
@@ -970,18 +436,6 @@
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
 ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="30000"/&gt;);
 PushConfigxml;</t>
   </si>
   <si>
@@ -1439,6 +893,546 @@
 PullConfigxml;
 ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
 ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_fullscreen=webview_xpath,true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_fullscreen=webview_xpath,false
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+EnterData(SettingPwdenter_xpath,1234);
+ClickNativeIcon(SettingsPwdOK_xpath);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+EnterData(SettingPwdenter_xpath,12345678910112233445566666);
+ClickNativeIcon(SettingsPwdOK_xpath);
+CheckUITextContains(password_wrong);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+EnterData(SettingPwdenter_xpath,4321);
+ClickNativeIcon(SettingsPwdOK_xpath);
+CheckUITextContains(password_wrong);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+ClickNativeIcon(SettingsPwdOK_xpath);
+CheckUITextContains(password_wrong);
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+ClickNativeIcon(SettingPwd_cancel_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(HomeButton_xpath);
+validate1;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://www.google.com);
+ClickNativeIcon(GoButton_xpath);
+SwitchApp(WEBVIEW);
+wait(8);
+validate1;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+link_Click(PBAndroid_test_link);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(BackButton_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(BackButton_xpath);
+ClickNativeIcon(ForwardButton_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SipButton_xpath);
+TakeScreenshot(VT187-012);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(ZoomtextButton_xpath);
+ClickNativeIcon(ZoomtextButton_xpath);
+TakeScreenshot(VT187-013);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(MinimizeButton_xpath);
+validate_AppMinimized(appsscreen);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+wait(4);
+CheckUITextContains(Establishing_Connection...);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+wait(4);
+CheckUITextContains(voidConnection);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="30000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+PullConfigxml;
+PullBkpConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/zoompage.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="1.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-008);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Signal~left:20semicolontop:300semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-003);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/zoompage.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="2.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-004);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/zoompage.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="3.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-005);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/zoompage.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="4.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-006);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/zoompage.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="-1.0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-009);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Battery~left:10semicolontop:200semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-007);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="SignatureCapture~left:30semicolontop:130semicolonheight:100semicolonbgcolor:#663300semicolonwidth:200semicolonborder:visiblesemicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(2);
+TakeScreenshot(VT187-011);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+EnterData(ExitPwdenter_xpath,1234);
+ClickNativeIcon(PwdOK_xpath);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate2
+{
+validate_Screenshot=VT187-007
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate2
+{
+validate_Screenshot=VT187-008
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate2
+{
+validate_Screenshot=VT187-009
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate2
+{
+validate_Screenshot=VT187-010
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+EnterData(ExitPwdenter_xpath,12345678910112233333454455666755555);
+ClickNativeIcon(PwdOK_xpath);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+ClickNativeIcon(PwdOK_xpath);
+CheckUITextContains(Invalid_Password);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+ClickNativeIcon(ExitPwd_cancel_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate2
+{
+validate_isIconDisplayed=SettingsButton_xpath,true
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Welcome to Enterprise Browser
+};
+validate2
+{
+validate_isIconDisplayed=SettingsButton_xpath,false
+};</t>
+  </si>
+  <si>
+    <t>wait(8);
+validate1;
+TakeScreenshot(VT187-010);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/SplashScreen,SplashScreenPath,&lt;SplashScreenPath value="file://%INSTALLDIR%/images/moto.png"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-011
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+EnterData(ExitPwdenter_xpath,4321);
+ClickNativeIcon(PwdOK_xpath);
+CheckUITextContains(Invalid_Password);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
 PushConfigxml;</t>
   </si>
 </sst>
@@ -1931,7 +1925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1983,7 +1979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" ht="90" thickBot="1">
+    <row r="2" spans="1:16384" ht="102.75" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2003,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -2032,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2061,10 +2057,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
@@ -39605,7 +39601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" ht="102.75" thickBot="1">
+    <row r="5" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -39625,16 +39621,16 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:16384" ht="102.75" thickBot="1">
+    <row r="6" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -39654,16 +39650,16 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:16384" ht="102.75" thickBot="1">
+    <row r="7" spans="1:16384" ht="128.25" thickBot="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -39683,16 +39679,16 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:16384" ht="102.75" thickBot="1">
+    <row r="8" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -39712,16 +39708,16 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:16384" ht="102.75" thickBot="1">
+    <row r="9" spans="1:16384" ht="128.25" thickBot="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -39741,16 +39737,16 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>111</v>
+        <v>152</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:16384" ht="102.75" thickBot="1">
+    <row r="10" spans="1:16384" ht="128.25" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -39770,10 +39766,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -39799,10 +39795,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>90</v>
+        <v>158</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39828,10 +39824,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>91</v>
+        <v>159</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -39857,16 +39853,16 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:16384" ht="128.25" thickBot="1">
+    <row r="14" spans="1:16384" ht="141" thickBot="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -39886,16 +39882,16 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:16384" ht="164.25" customHeight="1" thickBot="1">
+    <row r="15" spans="1:16384" ht="166.5" thickBot="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -39915,10 +39911,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39944,10 +39940,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39967,22 +39963,22 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="217.5" thickBot="1">
+    <row r="18" spans="1:11" ht="204.75" thickBot="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -40002,10 +39998,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>51</v>
+        <v>162</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -40025,22 +40021,22 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="192" thickBot="1">
+    <row r="20" spans="1:11" ht="179.25" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -40054,16 +40050,16 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>103</v>
+        <v>166</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -40089,10 +40085,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>37</v>
+        <v>168</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -40118,16 +40114,16 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="230.25" thickBot="1">
+    <row r="23" spans="1:11" ht="217.5" thickBot="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -40141,22 +40137,22 @@
         <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="243" thickBot="1">
+    <row r="24" spans="1:11" ht="217.5" thickBot="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -40170,22 +40166,22 @@
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>48</v>
+        <v>130</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="243" thickBot="1">
+    <row r="25" spans="1:11" ht="217.5" thickBot="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -40199,22 +40195,22 @@
         <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="179.25" thickBot="1">
+    <row r="26" spans="1:11" ht="153.75" thickBot="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -40228,22 +40224,22 @@
         <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="192" thickBot="1">
+    <row r="27" spans="1:11" ht="179.25" thickBot="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -40257,22 +40253,22 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="166.5" thickBot="1">
+    <row r="28" spans="1:11" ht="141" thickBot="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -40286,22 +40282,22 @@
         <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="204.75" thickBot="1">
+    <row r="29" spans="1:11" ht="192" thickBot="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -40315,22 +40311,22 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="179.25" thickBot="1">
+    <row r="30" spans="1:11" ht="166.5" thickBot="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -40344,22 +40340,22 @@
         <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="204.75" thickBot="1">
+    <row r="31" spans="1:11" ht="179.25" thickBot="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -40373,22 +40369,22 @@
         <v>10</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="179.25" thickBot="1">
+    <row r="32" spans="1:11" ht="153.75" thickBot="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -40402,22 +40398,22 @@
         <v>10</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="192" thickBot="1">
+    <row r="33" spans="1:11" ht="166.5" thickBot="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -40431,22 +40427,22 @@
         <v>10</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="128.25" thickBot="1">
+    <row r="34" spans="1:11" ht="115.5" thickBot="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -40460,22 +40456,22 @@
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="102.75" thickBot="1">
+    <row r="35" spans="1:11" ht="90" thickBot="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -40489,22 +40485,22 @@
         <v>10</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="128.25" thickBot="1">
+    <row r="36" spans="1:11" ht="115.5" thickBot="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -40518,22 +40514,22 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="141" thickBot="1">
+    <row r="37" spans="1:11" ht="128.25" thickBot="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -40547,16 +40543,16 @@
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -40576,16 +40572,16 @@
         <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -40605,16 +40601,16 @@
         <v>10</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -40634,16 +40630,16 @@
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -40663,16 +40659,16 @@
         <v>10</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -40692,16 +40688,16 @@
         <v>10</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -40721,16 +40717,16 @@
         <v>10</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -40750,16 +40746,16 @@
         <v>10</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -40779,16 +40775,16 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -40808,16 +40804,16 @@
         <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -40837,16 +40833,16 @@
         <v>10</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -40866,16 +40862,16 @@
         <v>10</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -40895,16 +40891,16 @@
         <v>10</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -40924,16 +40920,16 @@
         <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -40953,16 +40949,16 @@
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -40982,16 +40978,16 @@
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="F52" s="1">
         <v>1</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -41011,16 +41007,16 @@
         <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -41040,16 +41036,16 @@
         <v>10</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>151</v>
+        <v>105</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -41069,16 +41065,16 @@
         <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -41098,16 +41094,16 @@
         <v>10</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>154</v>
+        <v>108</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -41127,16 +41123,16 @@
         <v>10</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="204.75" thickBot="1">
@@ -41153,16 +41149,16 @@
         <v>10</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>158</v>
+        <v>112</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="268.5" thickBot="1">
@@ -41179,16 +41175,16 @@
         <v>10</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="128.25" thickBot="1">
@@ -41205,16 +41201,16 @@
         <v>10</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="F60" s="1">
         <v>1</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="128.25" thickBot="1">
@@ -41231,16 +41227,16 @@
         <v>10</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="128.25" thickBot="1">
@@ -41257,16 +41253,16 @@
         <v>10</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="F62" s="1">
         <v>1</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="115.5" thickBot="1">
@@ -41283,16 +41279,16 @@
         <v>10</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="F63" s="1">
         <v>1</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding apd RE22 and PB tests to automation
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7403" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7402" uniqueCount="175">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -1140,16 +1140,6 @@
 };
 validate2
 {
-validate_Screenshot=VT187-007
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Welcome to Enterprise Browser
-};
-validate2
-{
 validate_Screenshot=VT187-008
 };</t>
   </si>
@@ -1438,14 +1428,21 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>wait(4);
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
 ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
 PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_Screenshot=VT187-007
+};</t>
   </si>
 </sst>
 </file>
@@ -1937,9 +1934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2011,15 +2006,13 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>174</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:16384" ht="217.5" thickBot="1">
@@ -39812,7 +39805,7 @@
         <v>145</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39841,7 +39834,7 @@
         <v>136</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -39870,7 +39863,7 @@
         <v>144</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -39896,10 +39889,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -39928,7 +39921,7 @@
         <v>146</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39957,7 +39950,7 @@
         <v>147</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39983,10 +39976,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -40012,10 +40005,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -40041,10 +40034,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -40070,10 +40063,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -40099,10 +40092,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -40128,10 +40121,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>161</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -40160,7 +40153,7 @@
         <v>125</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -40186,10 +40179,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -40215,10 +40208,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -40244,10 +40237,10 @@
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -40418,7 +40411,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>69</v>
@@ -40476,10 +40469,10 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -40677,7 +40670,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>72</v>
@@ -40793,7 +40786,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>54</v>
@@ -41196,7 +41189,7 @@
         <v>112</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="128.25" thickBot="1">

</xml_diff>

<commit_message>
Adding screen shots in reference folder, fixed config issues
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7402" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7364" uniqueCount="170">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -185,17 +185,6 @@
     <t>Forward Debug Button</t>
   </si>
   <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Sanity specs
-};
-validate2
-{
-validate_PageTitle=Sanity specs
-};
-</t>
-  </si>
-  <si>
     <t>SIP Debug Button</t>
   </si>
   <si>
@@ -203,15 +192,6 @@
   </si>
   <si>
     <t>Minimize Debug Button</t>
-  </si>
-  <si>
-    <t>Void Connection Enabled</t>
-  </si>
-  <si>
-    <t>Void Connection Timeout</t>
-  </si>
-  <si>
-    <t>Void Connection Disbaled</t>
   </si>
   <si>
     <t>validate1
@@ -225,17 +205,6 @@
   </si>
   <si>
     <t>HourGlass Enabled</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="1" /&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>validate1
@@ -259,30 +228,6 @@
   </si>
   <si>
     <t>HourGlass Disabled</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(2);
-SwitchApp(NATIVE_APP);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(2);
-SwitchApp(NATIVE_APP);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>ServerCookie Validation</t>
@@ -408,18 +353,6 @@
     <t>User defined Navigation Timeout value</t>
   </si>
   <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>Default Navigation Timeout badlink file</t>
   </si>
   <si>
@@ -436,32 +369,7 @@
 };</t>
   </si>
   <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/abcd.html"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>Invalid Navigation Timeout value</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(32);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="-100"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>Invalid Navigation Timeout badlink file</t>
@@ -477,43 +385,7 @@
 }</t>
   </si>
   <si>
-    <t>wait(6);
-validate1;
-link_Click(ServerCookie_test_link);
-SwitchApp(NATIVE_APP);
-TypeinAddressbar(Addressbar_xpath,http://10.233.85.82:9097/1_Browser_Validation/cookie/servercookie.php?set=yes);
-ClickNativeIcon(GoButton_xpath);
-ClickNativeIcon(GoButton_xpath);
-ClickNativeIcon(ReloadButton_xpath);
-SwitchApp(WEBVIEW);
-wait(4);
-validate2;
-wait(4);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2679 - check the message box after resume the device with HostURL set  other device ip address in config with default Timeoutvalue</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="http://www.google.com"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Connecting to Google.."/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>validate1
@@ -533,262 +405,40 @@
     <t>VT187-2676 - check the message box after resume the device with HostURL set in config with default Timeoutvalue</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Connecting_to_Google..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9095"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2680 - check the message box after resume the device with HostURL set  other device ip address with port set to 9097 in config with default Timeoutvalue</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9097"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="wait till connection successfull"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>VT187-2681 - check the message box after resume the device with HostURL set  other device ip address with port set to 9095 in config with default Timeoutvalue</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(wait_till_connection_successfull);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="127.0.0.1"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2682 - check the message box after resume the device with HostURL set  other device ip address in config with default Timeoutvalue</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="111.222.11.00"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>VT187-2683 - check the message box after resume the device with HostURL set  ip address which does not exists in config with default Timeoutvalue</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(25);
-validate3;
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="60000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2685 - check the message box after resume the device with message set and  Timeoutvalue set to 60 seconds</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate2;
-wait(40);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="15000"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>VT187-2686 - check the message box after resume the device with message set and   Timeoutvalue set to 15 seconds</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="5000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2687 - check the message box after resume the device with message set and   Timeoutvalue set to 5 seconds</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="0"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>VT187-2688 - check the message box after resume the device with message set and   Timeoutvalue set to 0 seconds</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="-15000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2689 - check the message box after resume the device with Timeoutvalue set to -15  seconds</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout, );
-PushConfigxml;</t>
   </si>
   <si>
     <t>VT187-2684 - check the message box after resume the device without Timeoutvalue tag default value</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(back);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-2697 - message box on minimize and restore application</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(back);
-CheckUITextContains(Establishing_Connection..);
-press_Key(Home);
-wait(1);
-validate2;
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wifi_Mode(on);
-press_Key(back);
-wait(5);
-CheckUITextContains(voidConnection);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,TrackConnection,&lt;TrackConnection value="0" /&gt;);
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="1"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-0660 - Preload with NPAPI plugin PreloadLegacyGeneric</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>validate1
@@ -827,27 +477,7 @@
     <t>VT187-0670 - Preload with NPAPI plugin PreloadJSObjects</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>VT187-0671 - Do not Preload with NPAPI plugin PreloadJSObjects</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>validate1
@@ -883,116 +513,6 @@
 ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
 PushConfigxml;
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-ClickNativeIcon(SettingPwd_cancel_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t>wait(6);
-link_Click(PBAndroid_test_link);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(HomeButton_xpath);
-validate1;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-TypeinAddressbar(Addressbar_xpath,http://www.google.com);
-ClickNativeIcon(GoButton_xpath);
-SwitchApp(WEBVIEW);
-wait(8);
-validate1;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(BackButton_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(BackButton_xpath);
-ClickNativeIcon(ForwardButton_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(ZoomtextButton_xpath);
-ClickNativeIcon(ZoomtextButton_xpath);
-TakeScreenshot(VT187-013);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-wait(4);
-CheckUITextContains(Establishing_Connection...);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="0"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-wait(4);
-CheckUITextContains(voidConnection);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="30000"/&gt;);
-PushConfigxml;</t>
   </si>
   <si>
     <t>wait(4);
@@ -1191,20 +711,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(QuitButton_xpath);
-ClickNativeIcon(PwdOK_xpath);
-CheckUITextContains(Invalid_Password);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t>wait(6);
 validate1;
 SwitchApp(NATIVE_APP);
@@ -1308,17 +814,6 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(MinimizeButton_xpath);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=All Index
@@ -1375,59 +870,6 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-ClickNativeIcon(SettingsPwdOK_xpath);
-CheckUITextContains(password_wrong);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-wait(4);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/menu.html"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-wait(4);
-CheckUITextContains(Establishing_Connection...);
-wait(20);
-validate2;
-wait(4);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9097/1_Browser_Validation/cookie/" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SipButton_xpath);
-TakeScreenshot(VT187-012);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>wait(4);
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
@@ -1443,6 +885,581 @@
 {
 validate_Screenshot=VT187-007
 };</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+ClickNativeIcon(PwdOK_xpath);
+CheckUITextContains(Invalid_Password);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+ClickNativeIcon(SettingsPwdOK_xpath);
+CheckUITextContains(password_wrong);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Settings,SettingsButtonEnabled, &lt;SettingsButtonEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPageProtectionEnabled,&lt;SettingsPageProtectionEnabled value="1"/&gt;);
+ChangeConfigxml(Configuration/Settings,SettingsPagePassword, &lt;SettingsPagePassword value="1234"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+ClickNativeIcon(SettingPwd_cancel_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(HomeButton_xpath);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://www.google.com);
+ClickNativeIcon(GoButton_xpath);
+SwitchApp(WEBVIEW);
+wait(30);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+link_Click(PBAndroid_test_link);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(BackButton_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Sanity specs
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(BackButton_xpath);
+ClickNativeIcon(ForwardButton_xpath);
+SwitchApp(WEBVIEW);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SipButton_xpath);
+TakeScreenshot(VT187-012);
+validate2;
+PullConfigxml;
+PushBkpConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(ZoomtextButton_xpath);
+ClickNativeIcon(ZoomtextButton_xpath);
+TakeScreenshot(VT187-013);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(MinimizeButton_xpath);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(50);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="30000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(35);
+validate2;
+wait(4);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="-100"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/abcd.html"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate1;
+wait(4);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/menu.html"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="1" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+SwitchApp(NATIVE_APP);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+SwitchApp(NATIVE_APP);
+validate2;
+wait(4);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9097/1_Browser_Validation/cookie/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(ServerCookie_test_link);
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://10.233.85.82:9097/1_Browser_Validation/cookie/servercookie.php?set=yes);
+ClickNativeIcon(GoButton_xpath);
+ClickNativeIcon(ReloadButton_xpath);
+SwitchApp(WEBVIEW);
+wait(4);
+validate2;
+wait(4);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="http://www.google.com"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Connecting to Google.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Connecting_to_Google..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9095"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9097"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="wait till connection successfull"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(wait_till_connection_successfull);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="127.0.0.1"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="111.222.11.00"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(25);
+validate3;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="60000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate2;
+wait(40);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="15000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="5000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="-15000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout, );
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+press_Key(Home);
+wait(1);
+validate2;
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+wait(5);
+CheckUITextContains(voidConnection);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+validate2;
+PushBkpConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1932,9 +1949,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD63"/>
+  <dimension ref="A1:XFD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1996,9 +2015,7 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2006,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -2025,9 +2042,7 @@
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
@@ -2035,10 +2050,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2054,9 +2069,7 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
@@ -2064,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
@@ -39618,9 +39631,7 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="3" t="s">
         <v>33</v>
       </c>
@@ -39628,10 +39639,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -39647,9 +39658,7 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
@@ -39657,10 +39666,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -39676,9 +39685,7 @@
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
@@ -39686,10 +39693,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -39705,9 +39712,7 @@
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
@@ -39715,10 +39720,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -39734,9 +39739,7 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
@@ -39744,10 +39747,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -39763,9 +39766,7 @@
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
@@ -39773,10 +39774,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -39792,9 +39793,7 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
@@ -39802,10 +39801,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39821,9 +39820,7 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
@@ -39831,10 +39828,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -39850,9 +39847,7 @@
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="3" t="s">
         <v>24</v>
       </c>
@@ -39860,10 +39855,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -39879,9 +39874,7 @@
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
@@ -39889,10 +39882,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -39908,9 +39901,7 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="3" t="s">
         <v>26</v>
       </c>
@@ -39918,10 +39909,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39937,9 +39928,7 @@
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
@@ -39947,10 +39936,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39966,9 +39955,7 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="3" t="s">
         <v>39</v>
       </c>
@@ -39976,10 +39963,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -39995,9 +39982,7 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="3" t="s">
         <v>28</v>
       </c>
@@ -40005,16 +39990,16 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="179.25" thickBot="1">
+    <row r="19" spans="1:11" ht="204.75" thickBot="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -40024,9 +40009,7 @@
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="3" t="s">
         <v>37</v>
       </c>
@@ -40034,10 +40017,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -40053,20 +40036,18 @@
       <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -40082,9 +40063,7 @@
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="3" t="s">
         <v>29</v>
       </c>
@@ -40092,10 +40071,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -40111,9 +40090,7 @@
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="3" t="s">
         <v>30</v>
       </c>
@@ -40121,10 +40098,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -40140,9 +40117,7 @@
       <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="3" t="s">
         <v>35</v>
       </c>
@@ -40150,10 +40125,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -40169,9 +40144,7 @@
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
@@ -40179,10 +40152,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -40198,9 +40171,7 @@
       <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="3" t="s">
         <v>36</v>
       </c>
@@ -40208,16 +40179,16 @@
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="166.5" thickBot="1">
+    <row r="26" spans="1:11" ht="243" thickBot="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -40237,16 +40208,16 @@
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="179.25" thickBot="1">
+    <row r="27" spans="1:11" ht="192" thickBot="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -40260,22 +40231,22 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="141" thickBot="1">
+    <row r="28" spans="1:11" ht="153.75" thickBot="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -40295,7 +40266,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>42</v>
@@ -40304,7 +40275,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="192" thickBot="1">
+    <row r="29" spans="1:11" ht="204.75" thickBot="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -40324,7 +40295,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>34</v>
@@ -40333,7 +40304,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="166.5" thickBot="1">
+    <row r="30" spans="1:11" ht="179.25" thickBot="1">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -40353,7 +40324,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>45</v>
@@ -40362,7 +40333,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="179.25" thickBot="1">
+    <row r="31" spans="1:11" ht="192" thickBot="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -40382,10 +40353,10 @@
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -40405,22 +40376,22 @@
         <v>10</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="166.5" thickBot="1">
+    <row r="33" spans="1:11" ht="179.25" thickBot="1">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -40434,22 +40405,22 @@
         <v>10</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="115.5" thickBot="1">
+    <row r="34" spans="1:11" ht="153.75" thickBot="1">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -40463,22 +40434,22 @@
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="90" thickBot="1">
+    <row r="35" spans="1:11" ht="141" thickBot="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -40488,24 +40459,26 @@
       <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E35" s="3" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="115.5" thickBot="1">
+    <row r="36" spans="1:11" ht="153.75" thickBot="1">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -40519,22 +40492,22 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="128.25" thickBot="1">
+    <row r="37" spans="1:11" ht="141" thickBot="1">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -40548,22 +40521,22 @@
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="141" thickBot="1">
+    <row r="38" spans="1:11" ht="166.5" thickBot="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -40577,22 +40550,22 @@
         <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="141" thickBot="1">
+    <row r="39" spans="1:11" ht="179.25" thickBot="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -40606,22 +40579,22 @@
         <v>10</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>76</v>
+        <v>149</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="166.5" thickBot="1">
+    <row r="40" spans="1:11" ht="128.25" thickBot="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -40635,22 +40608,22 @@
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="179.25" thickBot="1">
+    <row r="41" spans="1:11" ht="128.25" thickBot="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -40664,22 +40637,22 @@
         <v>10</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="128.25" thickBot="1">
+    <row r="42" spans="1:11" ht="166.5" thickBot="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -40693,22 +40666,22 @@
         <v>10</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="141" thickBot="1">
+    <row r="43" spans="1:11" ht="217.5" thickBot="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -40728,16 +40701,16 @@
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="128.25" thickBot="1">
+    <row r="44" spans="1:11" ht="281.25" thickBot="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -40751,22 +40724,22 @@
         <v>10</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>61</v>
+        <v>155</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="179.25" thickBot="1">
+    <row r="45" spans="1:11" ht="268.5" thickBot="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -40780,16 +40753,16 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -40809,22 +40782,22 @@
         <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="217.5" thickBot="1">
+    <row r="47" spans="1:11" ht="268.5" thickBot="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -40838,22 +40811,22 @@
         <v>10</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="204.75" thickBot="1">
+    <row r="48" spans="1:11" ht="268.5" thickBot="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -40867,16 +40840,16 @@
         <v>10</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -40896,22 +40869,22 @@
         <v>10</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="204.75" thickBot="1">
+    <row r="50" spans="1:11" ht="306.75" thickBot="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -40925,22 +40898,22 @@
         <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="204.75" thickBot="1">
+    <row r="51" spans="1:11" ht="281.25" thickBot="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -40954,22 +40927,22 @@
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" ht="166.5" thickBot="1">
+    <row r="52" spans="1:11" ht="243" thickBot="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -40983,22 +40956,22 @@
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="F52" s="1">
         <v>1</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" ht="243" thickBot="1">
+    <row r="53" spans="1:11" ht="281.25" thickBot="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -41012,22 +40985,22 @@
         <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="217.5" thickBot="1">
+    <row r="54" spans="1:11" ht="281.25" thickBot="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -41041,22 +41014,19 @@
         <v>10</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
+        <v>76</v>
+      </c>
     </row>
-    <row r="55" spans="1:11" ht="217.5" thickBot="1">
+    <row r="55" spans="1:11" ht="268.5" thickBot="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -41070,22 +41040,19 @@
         <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
+        <v>76</v>
+      </c>
     </row>
-    <row r="56" spans="1:11" ht="217.5" thickBot="1">
+    <row r="56" spans="1:11" ht="294" thickBot="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -41099,22 +41066,19 @@
         <v>10</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
+        <v>128</v>
+      </c>
     </row>
-    <row r="57" spans="1:11" ht="217.5" thickBot="1">
+    <row r="57" spans="1:11" ht="141" thickBot="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -41128,23 +41092,23 @@
         <v>10</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="204.75" thickBot="1">
+    <row r="58" spans="1:11" ht="128.25" thickBot="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="11">
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -41153,20 +41117,20 @@
       <c r="D58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>109</v>
+      <c r="E58" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
       </c>
-      <c r="G58" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>88</v>
+      <c r="G58" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="268.5" thickBot="1">
+    <row r="59" spans="1:11" ht="141" thickBot="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -41180,23 +41144,23 @@
         <v>10</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>112</v>
+        <v>168</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>166</v>
+        <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="128.25" thickBot="1">
+    <row r="60" spans="1:11" ht="115.5" thickBot="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="11">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -41205,95 +41169,17 @@
       <c r="D60" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>113</v>
+      <c r="E60" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="F60" s="1">
         <v>1</v>
       </c>
-      <c r="G60" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="128.25" thickBot="1">
-      <c r="A61" s="1">
-        <v>60</v>
-      </c>
-      <c r="B61" s="11">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H61" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="128.25" thickBot="1">
-      <c r="A62" s="1">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F62" s="1">
-        <v>1</v>
-      </c>
-      <c r="G62" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="115.5" thickBot="1">
-      <c r="A63" s="1">
-        <v>62</v>
-      </c>
-      <c r="B63" s="11">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" s="1">
-        <v>1</v>
-      </c>
-      <c r="G63" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="H63" s="13" t="s">
-        <v>118</v>
+      <c r="G60" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added automatable to config.xls file
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7364" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="170">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -1952,7 +1952,7 @@
   <dimension ref="A1:XFD60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2015,7 +2015,9 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2042,7 +2044,9 @@
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
@@ -2069,7 +2073,9 @@
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
@@ -39631,7 +39637,9 @@
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>33</v>
       </c>
@@ -39658,7 +39666,9 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
@@ -39685,7 +39695,9 @@
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
@@ -39712,7 +39724,9 @@
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
@@ -39739,7 +39753,9 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
@@ -39766,7 +39782,9 @@
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
@@ -39793,7 +39811,9 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>32</v>
       </c>
@@ -39820,7 +39840,9 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
@@ -39847,7 +39869,9 @@
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>24</v>
       </c>
@@ -39874,7 +39898,9 @@
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
@@ -39901,7 +39927,9 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E15" s="3" t="s">
         <v>26</v>
       </c>
@@ -39928,7 +39956,9 @@
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
@@ -39955,7 +39985,9 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E17" s="3" t="s">
         <v>39</v>
       </c>
@@ -39982,7 +40014,9 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E18" s="3" t="s">
         <v>28</v>
       </c>
@@ -40009,7 +40043,9 @@
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E19" s="3" t="s">
         <v>37</v>
       </c>
@@ -40036,7 +40072,9 @@
       <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E20" s="3" t="s">
         <v>56</v>
       </c>
@@ -40063,7 +40101,9 @@
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E21" s="3" t="s">
         <v>29</v>
       </c>
@@ -40090,7 +40130,9 @@
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>30</v>
       </c>
@@ -40117,7 +40159,9 @@
       <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>35</v>
       </c>
@@ -40144,7 +40188,9 @@
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
@@ -40171,7 +40217,9 @@
       <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E25" s="3" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Fixed issues in config DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -131,13 +131,6 @@
     <t xml:space="preserve">FullScreenDisabled </t>
   </si>
   <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Google
-};
-</t>
-  </si>
-  <si>
     <t>SettingsButtonProtection password</t>
   </si>
   <si>
@@ -157,13 +150,6 @@
   </si>
   <si>
     <t>Home Debug Button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=All Index
-};
-</t>
   </si>
   <si>
     <t>Go Debug Button</t>
@@ -918,49 +904,6 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SettingsButton_xpath);
-ClickNativeIcon(SettingPwd_cancel_xpath);
-SwitchApp(WEBVIEW);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;
-</t>
-  </si>
-  <si>
-    <t>wait(6);
-link_Click(PBAndroid_test_link);
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(HomeButton_xpath);
-validate1;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-link_Click(PBAndroid_test_link);
-validate1;
-SwitchApp(NATIVE_APP);
-TypeinAddressbar(Addressbar_xpath,http://www.google.com);
-ClickNativeIcon(GoButton_xpath);
-SwitchApp(WEBVIEW);
-wait(30);
-validate1;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>wait(4);
 link_Click(PBAndroid_test_link);
 validate1;
@@ -1106,310 +1049,6 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="1" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-SwitchApp(NATIVE_APP);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-SwitchApp(NATIVE_APP);
-validate2;
-wait(4);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9097/1_Browser_Validation/cookie/" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(ServerCookie_test_link);
-SwitchApp(NATIVE_APP);
-TypeinAddressbar(Addressbar_xpath,http://10.233.85.82:9097/1_Browser_Validation/cookie/servercookie.php?set=yes);
-ClickNativeIcon(GoButton_xpath);
-ClickNativeIcon(ReloadButton_xpath);
-SwitchApp(WEBVIEW);
-wait(4);
-validate2;
-wait(4);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PullConfigxml;
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="0"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="http://www.google.com"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Connecting to Google.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Connecting_to_Google..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9095"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9097"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="wait till connection successfull"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(wait_till_connection_successfull);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="127.0.0.1"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="111.222.11.00"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(25);
-validate3;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="60000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate2;
-wait(40);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="15000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="5000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="-15000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Timeout, );
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-wifi_Mode(off);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-CheckUITextContains(Establishing_Connection..);
-wait(2);
-validate2;
-wait(15);
-validate3;
-wifi_Mode(on);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
-ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>wait(4);
 validate1;
 wifi_Mode(off);
@@ -1460,6 +1099,390 @@
 ClickRunTest(runtest_top_xpath);
 validate2;
 PushBkpConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://www.google.com);
+ClickNativeIcon(GoButton_xpath);
+SwitchApp(WEBVIEW);
+wait(30);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Google
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(6);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SettingsButton_xpath);
+ClickNativeIcon(SettingPwd_cancel_xpath);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=Sanity specs
+};</t>
+  </si>
+  <si>
+    <t>wait(6);
+link_Click(PBAndroid_test_link);
+wait(5);
+validate2;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(HomeButton_xpath);
+SwitchApp(WEBVIEW);
+wait(6);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+SwitchApp(NATIVE_APP);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="0" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="http://www.google.com"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Connecting to Google.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Connecting_to_Google..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9095"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82:9097"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="wait till connection successfull"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(wait_till_connection_successfull);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="127.0.0.1"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="111.222.11.00"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(25);
+validate3;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="60000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate2;
+wait(40);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="15000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="5000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="-15000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout, );
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+wifi_Mode(off);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+CheckUITextContains(Establishing_Connection..);
+wait(2);
+validate2;
+wait(15);
+validate3;
+wifi_Mode(on);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Timeout,  &lt;Timeout value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(48);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/GUI,HourglassEnabled, &lt;HourglassEnabled   value="1" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(ServerCookie_test_link);
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://10.233.85.82:9097/1_Browser_Validation/cookie/servercookie.php?set=yes);
+wait(2);
+ClickNativeIcon(GoButton_xpath);
+wait(4);
+ClickNativeIcon(ReloadButton_xpath);
+SwitchApp(WEBVIEW);
+wait(4);
+validate2;
+wait(4);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/VoidConnection,TrackConnection, &lt;TrackConnection value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,HostURL, &lt;HostURL value="10.233.85.82"/&gt;);
+ChangeConfigxml(Configuration/VoidConnection,Message, &lt;Message value="Establishing Connection.."/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+SwitchApp(NATIVE_APP);
+validate2;
+wait(4);
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9097/1_Browser_Validation/cookie/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+PushConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1951,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2025,7 +2048,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -2054,10 +2077,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2083,10 +2106,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
@@ -39647,10 +39670,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -39676,10 +39699,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -39705,10 +39728,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -39734,10 +39757,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -39763,10 +39786,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -39792,10 +39815,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -39821,10 +39844,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39850,10 +39873,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -39879,10 +39902,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -39908,10 +39931,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -39937,10 +39960,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39966,10 +39989,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39989,16 +40012,16 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -40024,10 +40047,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -40047,16 +40070,16 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -40076,16 +40099,16 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -40111,10 +40134,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -40140,10 +40163,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -40163,16 +40186,16 @@
         <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -40192,16 +40215,16 @@
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -40221,16 +40244,16 @@
         <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -40250,16 +40273,16 @@
         <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -40279,22 +40302,22 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="153.75" thickBot="1">
+    <row r="28" spans="1:11" ht="204.75" thickBot="1">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -40308,22 +40331,22 @@
         <v>10</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F28" s="1">
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>42</v>
+        <v>152</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="204.75" thickBot="1">
+    <row r="29" spans="1:11" ht="179.25" thickBot="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -40337,16 +40360,16 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -40366,16 +40389,16 @@
         <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -40395,16 +40418,16 @@
         <v>10</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -40424,16 +40447,16 @@
         <v>10</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -40453,16 +40476,16 @@
         <v>10</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -40482,16 +40505,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F34" s="1">
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -40511,16 +40534,16 @@
         <v>10</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -40540,16 +40563,16 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -40569,16 +40592,16 @@
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -40598,16 +40621,16 @@
         <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -40627,22 +40650,22 @@
         <v>10</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="128.25" thickBot="1">
+    <row r="40" spans="1:11" ht="153.75" thickBot="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -40656,22 +40679,22 @@
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="128.25" thickBot="1">
+    <row r="41" spans="1:11" ht="153.75" thickBot="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -40685,16 +40708,16 @@
         <v>10</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -40714,22 +40737,22 @@
         <v>10</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="217.5" thickBot="1">
+    <row r="43" spans="1:11" ht="294" thickBot="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -40743,22 +40766,22 @@
         <v>10</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="281.25" thickBot="1">
+    <row r="44" spans="1:11" ht="294" thickBot="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -40772,7 +40795,7 @@
         <v>10</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F44" s="1">
         <v>1</v>
@@ -40781,13 +40804,13 @@
         <v>155</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="268.5" thickBot="1">
+    <row r="45" spans="1:11" ht="281.25" thickBot="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -40801,7 +40824,7 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
@@ -40810,13 +40833,13 @@
         <v>156</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="268.5" thickBot="1">
+    <row r="46" spans="1:11" ht="281.25" thickBot="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -40830,7 +40853,7 @@
         <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
@@ -40839,13 +40862,13 @@
         <v>157</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="268.5" thickBot="1">
+    <row r="47" spans="1:11" ht="281.25" thickBot="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -40859,7 +40882,7 @@
         <v>10</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
@@ -40868,13 +40891,13 @@
         <v>158</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="268.5" thickBot="1">
+    <row r="48" spans="1:11" ht="281.25" thickBot="1">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -40888,7 +40911,7 @@
         <v>10</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
@@ -40897,13 +40920,13 @@
         <v>159</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="204.75" thickBot="1">
+    <row r="49" spans="1:11" ht="217.5" thickBot="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -40917,7 +40940,7 @@
         <v>10</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
@@ -40926,13 +40949,13 @@
         <v>160</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="306.75" thickBot="1">
+    <row r="50" spans="1:11" ht="319.5" thickBot="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -40946,7 +40969,7 @@
         <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
@@ -40955,13 +40978,13 @@
         <v>161</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="281.25" thickBot="1">
+    <row r="51" spans="1:11" ht="294" thickBot="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -40975,7 +40998,7 @@
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
@@ -40984,13 +41007,13 @@
         <v>162</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" ht="243" thickBot="1">
+    <row r="52" spans="1:11" ht="255.75" thickBot="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -41004,22 +41027,22 @@
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F52" s="1">
         <v>1</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" ht="281.25" thickBot="1">
+    <row r="53" spans="1:11" ht="294" thickBot="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -41033,7 +41056,7 @@
         <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
@@ -41042,13 +41065,13 @@
         <v>163</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="281.25" thickBot="1">
+    <row r="54" spans="1:11" ht="294" thickBot="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -41062,7 +41085,7 @@
         <v>10</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
@@ -41071,10 +41094,10 @@
         <v>164</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="268.5" thickBot="1">
+    <row r="55" spans="1:11" ht="281.25" thickBot="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -41088,7 +41111,7 @@
         <v>10</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -41097,7 +41120,7 @@
         <v>165</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="294" thickBot="1">
@@ -41114,16 +41137,16 @@
         <v>10</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="141" thickBot="1">
@@ -41140,16 +41163,16 @@
         <v>10</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="128.25" thickBot="1">
@@ -41166,16 +41189,16 @@
         <v>10</v>
       </c>
       <c r="E58" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H58" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="F58" s="1">
-        <v>1</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="141" thickBot="1">
@@ -41192,16 +41215,16 @@
         <v>10</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="115.5" thickBot="1">
@@ -41218,16 +41241,16 @@
         <v>10</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F60" s="1">
         <v>1</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues in DSL in device and application
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7388" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7383" uniqueCount="167">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>PageZoomEnabled as 4.0</t>
-  </si>
-  <si>
-    <t>PageZoomEnabled as -1.0</t>
   </si>
   <si>
     <t xml:space="preserve">FullScreenDisabled </t>
@@ -287,16 +284,6 @@
 validate2
 {
 validate_Screenshot=VT187-006
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-012
 };</t>
   </si>
   <si>
@@ -585,32 +572,11 @@
   <si>
     <t>wait(6);
 validate1;
-TakeScreenshot(VT187-006);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/zoompage.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Screen,PageZoom,&lt;PageZoom value="-1.0" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
 TakeScreenshot(VT187-009);
 validate2;
 PushBkpConfigxml;
 PullConfigxml;
 ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="Battery~left:10semicolontop:200semicoloncolor:#663300semicolonvisibility:visible"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-TakeScreenshot(VT187-007);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="SignatureCapture~left:30semicolontop:130semicolonheight:100semicolonbgcolor:#663300semicolonwidth:200semicolonborder:visiblesemicolonvisibility:visible"/&gt;);
 PushConfigxml;</t>
   </si>
   <si>
@@ -863,16 +829,6 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-007
-};</t>
-  </si>
-  <si>
     <t xml:space="preserve">wait(6);
 validate1;
 SwitchApp(NATIVE_APP);
@@ -934,19 +890,6 @@
 validate1;
 PushBkpConfigxml;
 PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(SipButton_xpath);
-TakeScreenshot(VT187-012);
-validate2;
-PullConfigxml;
-PushBkpConfigxml;
 ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
 PushConfigxml;</t>
@@ -1484,6 +1427,38 @@
 ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
 PushConfigxml;</t>
   </si>
+  <si>
+    <t>wait(6);
+validate1;
+TakeScreenshot(VT187-006);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DefaultMetaTags,MetaTag,&lt;MetaTag VALUE="SignatureCapture~left:30semicolontop:130semicolonheight:100semicolonbgcolor:#663300semicolonwidth:200semicolonborder:visiblesemicolonvisibility:visible"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+textBoxClick(SipButton_xpath);
+sendKeyEvents(a);
+validate2;
+PullConfigxml;
+PushBkpConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_textBoxData=SipButton_xpath,a
+};</t>
+  </si>
 </sst>
 </file>
 
@@ -1972,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD60"/>
+  <dimension ref="A1:XFD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2048,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -2077,10 +2052,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -2106,10 +2081,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
@@ -39664,16 +39639,16 @@
         <v>10</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -39699,10 +39674,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -39728,10 +39703,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -39757,10 +39732,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -39786,10 +39761,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -39815,18 +39790,18 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:16384" ht="128.25" thickBot="1">
+    <row r="11" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -39838,16 +39813,16 @@
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39855,7 +39830,7 @@
     </row>
     <row r="12" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -39867,24 +39842,24 @@
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:16384" ht="115.5" thickBot="1">
+    <row r="13" spans="1:16384" ht="141" thickBot="1">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -39896,24 +39871,24 @@
         <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:16384" ht="141" thickBot="1">
+    <row r="14" spans="1:16384" ht="166.5" thickBot="1">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -39925,24 +39900,24 @@
         <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:16384" ht="166.5" thickBot="1">
+    <row r="15" spans="1:16384" ht="192" thickBot="1">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -39954,16 +39929,16 @@
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39971,7 +39946,7 @@
     </row>
     <row r="16" spans="1:16384" ht="192" thickBot="1">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -39983,24 +39958,24 @@
         <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="192" thickBot="1">
+    <row r="17" spans="1:11" ht="204.75" thickBot="1">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -40012,16 +39987,16 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -40029,7 +40004,7 @@
     </row>
     <row r="18" spans="1:11" ht="204.75" thickBot="1">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -40041,24 +40016,24 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="204.75" thickBot="1">
+    <row r="19" spans="1:11" ht="179.25" thickBot="1">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -40070,24 +40045,24 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="179.25" thickBot="1">
+    <row r="20" spans="1:11" ht="128.25" thickBot="1">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -40099,24 +40074,24 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="128.25" thickBot="1">
+    <row r="21" spans="1:11" ht="166.5" thickBot="1">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -40128,24 +40103,24 @@
         <v>10</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="166.5" thickBot="1">
+    <row r="22" spans="1:11" ht="217.5" thickBot="1">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -40157,24 +40132,24 @@
         <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="217.5" thickBot="1">
+    <row r="23" spans="1:11" ht="230.25" thickBot="1">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -40186,16 +40161,16 @@
         <v>10</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -40203,7 +40178,7 @@
     </row>
     <row r="24" spans="1:11" ht="230.25" thickBot="1">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -40215,24 +40190,24 @@
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="230.25" thickBot="1">
+    <row r="25" spans="1:11" ht="243" thickBot="1">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -40244,24 +40219,24 @@
         <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="243" thickBot="1">
+    <row r="26" spans="1:11" ht="192" thickBot="1">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -40273,24 +40248,24 @@
         <v>10</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="192" thickBot="1">
+    <row r="27" spans="1:11" ht="204.75" thickBot="1">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -40302,24 +40277,24 @@
         <v>10</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="204.75" thickBot="1">
+    <row r="28" spans="1:11" ht="179.25" thickBot="1">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -40337,10 +40312,10 @@
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -40348,7 +40323,7 @@
     </row>
     <row r="29" spans="1:11" ht="179.25" thickBot="1">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -40366,18 +40341,18 @@
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="179.25" thickBot="1">
+    <row r="30" spans="1:11" ht="192" thickBot="1">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -40389,24 +40364,24 @@
         <v>10</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>43</v>
+        <v>129</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="192" thickBot="1">
+    <row r="31" spans="1:11" ht="153.75" thickBot="1">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
@@ -40424,18 +40399,18 @@
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="166.5" thickBot="1">
+    <row r="32" spans="1:11" ht="179.25" thickBot="1">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -40453,18 +40428,18 @@
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="179.25" thickBot="1">
+    <row r="33" spans="1:11" ht="153.75" thickBot="1">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -40482,18 +40457,18 @@
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="153.75" thickBot="1">
+    <row r="34" spans="1:11" ht="141" thickBot="1">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -40505,24 +40480,24 @@
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="141" thickBot="1">
+    <row r="35" spans="1:11" ht="153.75" thickBot="1">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
@@ -40534,24 +40509,24 @@
         <v>10</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="153.75" thickBot="1">
+    <row r="36" spans="1:11" ht="141" thickBot="1">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -40563,24 +40538,24 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="141" thickBot="1">
+    <row r="37" spans="1:11" ht="166.5" thickBot="1">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -40592,24 +40567,24 @@
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="166.5" thickBot="1">
+    <row r="38" spans="1:11" ht="179.25" thickBot="1">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -40621,24 +40596,24 @@
         <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>48</v>
+        <v>137</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="179.25" thickBot="1">
+    <row r="39" spans="1:11" ht="153.75" thickBot="1">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -40650,16 +40625,16 @@
         <v>10</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -40667,7 +40642,7 @@
     </row>
     <row r="40" spans="1:11" ht="153.75" thickBot="1">
       <c r="A40" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -40679,24 +40654,24 @@
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="153.75" thickBot="1">
+    <row r="41" spans="1:11" ht="166.5" thickBot="1">
       <c r="A41" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -40708,13 +40683,13 @@
         <v>10</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>50</v>
@@ -40723,9 +40698,9 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="166.5" thickBot="1">
+    <row r="42" spans="1:11" ht="294" thickBot="1">
       <c r="A42" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -40743,10 +40718,10 @@
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -40754,7 +40729,7 @@
     </row>
     <row r="43" spans="1:11" ht="294" thickBot="1">
       <c r="A43" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -40766,13 +40741,13 @@
         <v>10</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>72</v>
@@ -40781,9 +40756,9 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="294" thickBot="1">
+    <row r="44" spans="1:11" ht="281.25" thickBot="1">
       <c r="A44" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -40801,10 +40776,10 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -40812,7 +40787,7 @@
     </row>
     <row r="45" spans="1:11" ht="281.25" thickBot="1">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -40824,16 +40799,16 @@
         <v>10</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -40841,7 +40816,7 @@
     </row>
     <row r="46" spans="1:11" ht="281.25" thickBot="1">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -40853,16 +40828,16 @@
         <v>10</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F46" s="1">
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -40870,7 +40845,7 @@
     </row>
     <row r="47" spans="1:11" ht="281.25" thickBot="1">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -40882,24 +40857,24 @@
         <v>10</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="281.25" thickBot="1">
+    <row r="48" spans="1:11" ht="217.5" thickBot="1">
       <c r="A48" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -40911,24 +40886,24 @@
         <v>10</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="217.5" thickBot="1">
+    <row r="49" spans="1:11" ht="319.5" thickBot="1">
       <c r="A49" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -40940,24 +40915,24 @@
         <v>10</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="319.5" thickBot="1">
+    <row r="50" spans="1:11" ht="294" thickBot="1">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -40969,24 +40944,24 @@
         <v>10</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="294" thickBot="1">
+    <row r="51" spans="1:11" ht="255.75" thickBot="1">
       <c r="A51" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -40998,24 +40973,24 @@
         <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" ht="255.75" thickBot="1">
+    <row r="52" spans="1:11" ht="294" thickBot="1">
       <c r="A52" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
@@ -41027,16 +41002,16 @@
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F52" s="1">
         <v>1</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -41044,7 +41019,7 @@
     </row>
     <row r="53" spans="1:11" ht="294" thickBot="1">
       <c r="A53" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -41056,201 +41031,172 @@
         <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="281.25" thickBot="1">
+      <c r="A54" s="1">
+        <v>54</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F53" s="1">
-        <v>1</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="54" spans="1:11" ht="294" thickBot="1">
-      <c r="A54" s="1">
-        <v>53</v>
-      </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="3" t="s">
+    <row r="55" spans="1:11" ht="294" thickBot="1">
+      <c r="A55" s="1">
+        <v>55</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F54" s="1">
-        <v>1</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>74</v>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="281.25" thickBot="1">
-      <c r="A55" s="1">
-        <v>54</v>
-      </c>
-      <c r="B55" s="1">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="3" t="s">
+    <row r="56" spans="1:11" ht="141" thickBot="1">
+      <c r="A56" s="1">
+        <v>56</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F55" s="1">
-        <v>1</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>74</v>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="294" thickBot="1">
-      <c r="A56" s="1">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="3" t="s">
+    <row r="57" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A57" s="1">
+        <v>57</v>
+      </c>
+      <c r="B57" s="11">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="141" thickBot="1">
+      <c r="A58" s="1">
+        <v>58</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H58" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F56" s="1">
-        <v>1</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>126</v>
-      </c>
     </row>
-    <row r="57" spans="1:11" ht="141" thickBot="1">
-      <c r="A57" s="1">
-        <v>56</v>
-      </c>
-      <c r="B57" s="1">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="1">
-        <v>1</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="128.25" thickBot="1">
-      <c r="A58" s="1">
-        <v>57</v>
-      </c>
-      <c r="B58" s="11">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="12" t="s">
+    <row r="59" spans="1:11" ht="115.5" thickBot="1">
+      <c r="A59" s="1">
+        <v>59</v>
+      </c>
+      <c r="B59" s="11">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H59" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="F58" s="1">
-        <v>1</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="141" thickBot="1">
-      <c r="A59" s="1">
-        <v>58</v>
-      </c>
-      <c r="B59" s="1">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F59" s="1">
-        <v>1</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="H59" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="115.5" thickBot="1">
-      <c r="A60" s="1">
-        <v>59</v>
-      </c>
-      <c r="B60" s="11">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F60" s="1">
-        <v>1</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed PB and EB DSL issues
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -427,16 +427,6 @@
     <t>VT187-0661 - Do not Preload with NPAPI plugin PreloadLegacyGeneric</t>
   </si>
   <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="1"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=PB and RE2.2 Semi Auto Frame Work : SignatureCapture
@@ -580,18 +570,6 @@
 PushConfigxml;</t>
   </si>
   <si>
-    <t>wait(2);
-TakeScreenshot(VT187-011);
-validate1;
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
-ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
     <t>wait(6);
 validate1;
 SwitchApp(NATIVE_APP);
@@ -727,27 +705,6 @@
 validate2
 {
 validate_isIconDisplayed=SettingsButton_xpath,false
-};</t>
-  </si>
-  <si>
-    <t>wait(8);
-validate1;
-TakeScreenshot(VT187-010);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/SplashScreen,SplashScreenPath,&lt;SplashScreenPath value="file://%INSTALLDIR%/images/moto.png"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=All Index
-};
-validate2
-{
-validate_Screenshot=VT187-011
 };</t>
   </si>
   <si>
@@ -955,18 +912,6 @@
 PushBkpConfigxml;
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(48);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
 ChangeConfigxml(Configuration/Applications/Application/Navigation,BadLinkURI,&lt;BadLinkURI value="file://%INSTALLDIR%/abcd.html"/&gt;);
 ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
 PushConfigxml;</t>
@@ -1013,35 +958,6 @@
 ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="1"/&gt;);
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
 PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-validate2;
-PushBkpConfigxml;</t>
   </si>
   <si>
     <t>wait(6);
@@ -1438,10 +1354,41 @@
 PushConfigxml;</t>
   </si>
   <si>
+    <t>wait(8);
+validate1;
+TakeScreenshot(VT187-010);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/SplashScreen,SplashScreenPath,&lt;SplashScreenPath value="file://%INSTALLDIR%/images/moto.png"/&gt;);
+ChangeConfigxml(Configuration/SplashScreen,SplashScreenDuration,&lt;SplashScreenDuration value="8000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(2);
+TakeScreenshot(VT187-011);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordEnabled, &lt;ExitPasswordEnabled value="1" /&gt;);
+ChangeConfigxml(Configuration/ExitPassword,ExitPasswordValue, &lt;ExitPasswordValue value="1234" /&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>Validate2
+{
+validate_Screenshot=VT187-011
+};</t>
+  </si>
+  <si>
     <t>wait(6);
 validate1;
-textBoxClick(SipButton_xpath);
-sendKeyEvents(a);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(SipButton_xpath);
+wait(3);
+UIAutomatorScreenshot(VT187-012);
 validate2;
 PullConfigxml;
 PushBkpConfigxml;
@@ -1456,8 +1403,63 @@
 };
 validate2
 {
-validate_textBoxData=SipButton_xpath,a
+validate_Screenshot=VT187-012
 };</t>
+  </si>
+  <si>
+    <t>wait(6);
+validate1;
+link_Click(NavTimeOut_link);
+wait(60);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+wait(5);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+wait(5);
+validate2;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+wait(5);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="0"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>wait(4);
+validate1;
+ClickRunTest(runtest_top_xpath);
+wait(5);
+validate2;
+PushBkpConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1949,8 +1951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2023,7 +2025,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -2052,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>54</v>
@@ -2081,7 +2083,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>55</v>
@@ -39645,10 +39647,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -39674,10 +39676,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -39703,7 +39705,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>62</v>
@@ -39732,7 +39734,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>56</v>
@@ -39761,7 +39763,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>57</v>
@@ -39790,7 +39792,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>58</v>
@@ -39819,10 +39821,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39848,16 +39850,16 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:16384" ht="141" thickBot="1">
+    <row r="13" spans="1:16384" ht="166.5" thickBot="1">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -39877,16 +39879,16 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:16384" ht="166.5" thickBot="1">
+    <row r="14" spans="1:16384" ht="153.75" thickBot="1">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -39906,10 +39908,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>104</v>
+        <v>158</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -39935,10 +39937,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39964,10 +39966,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39993,10 +39995,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -40022,10 +40024,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -40051,10 +40053,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -40080,10 +40082,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -40109,10 +40111,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -40138,10 +40140,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -40167,10 +40169,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -40196,10 +40198,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -40225,10 +40227,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -40254,7 +40256,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>61</v>
@@ -40283,10 +40285,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -40312,10 +40314,10 @@
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -40341,7 +40343,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>42</v>
@@ -40370,16 +40372,16 @@
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="153.75" thickBot="1">
+    <row r="31" spans="1:11" ht="179.25" thickBot="1">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -40399,10 +40401,10 @@
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -40428,7 +40430,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>59</v>
@@ -40457,10 +40459,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -40486,7 +40488,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>47</v>
@@ -40515,7 +40517,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>47</v>
@@ -40544,7 +40546,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>47</v>
@@ -40573,7 +40575,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>47</v>
@@ -40602,10 +40604,10 @@
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -40631,7 +40633,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="H39" s="7" t="s">
         <v>67</v>
@@ -40660,7 +40662,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>49</v>
@@ -40689,7 +40691,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>50</v>
@@ -40718,7 +40720,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>70</v>
@@ -40747,7 +40749,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>72</v>
@@ -40776,7 +40778,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>72</v>
@@ -40805,7 +40807,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H45" s="7" t="s">
         <v>72</v>
@@ -40834,7 +40836,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>72</v>
@@ -40863,7 +40865,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>72</v>
@@ -40892,7 +40894,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="H48" s="7" t="s">
         <v>72</v>
@@ -40921,7 +40923,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>72</v>
@@ -40950,7 +40952,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H50" s="7" t="s">
         <v>72</v>
@@ -40979,7 +40981,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H51" s="7" t="s">
         <v>72</v>
@@ -41008,7 +41010,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H52" s="7" t="s">
         <v>72</v>
@@ -41037,7 +41039,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>72</v>
@@ -41063,7 +41065,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>72</v>
@@ -41089,13 +41091,13 @@
         <v>1</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="141" thickBot="1">
+    <row r="56" spans="1:11" ht="153.75" thickBot="1">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -41115,13 +41117,13 @@
         <v>1</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="H56" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="128.25" thickBot="1">
+    <row r="57" spans="1:11" ht="141" thickBot="1">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -41141,13 +41143,13 @@
         <v>1</v>
       </c>
       <c r="G57" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="H57" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H57" s="13" t="s">
-        <v>89</v>
-      </c>
     </row>
-    <row r="58" spans="1:11" ht="141" thickBot="1">
+    <row r="58" spans="1:11" ht="153.75" thickBot="1">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -41161,13 +41163,13 @@
         <v>10</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="H58" s="7" t="s">
         <v>86</v>
@@ -41187,16 +41189,16 @@
         <v>10</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed config issues in DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7383" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7358" uniqueCount="155">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -342,9 +342,6 @@
 };</t>
   </si>
   <si>
-    <t>Invalid Navigation Timeout value</t>
-  </si>
-  <si>
     <t>Invalid Navigation Timeout badlink file</t>
   </si>
   <si>
@@ -409,38 +406,6 @@
   </si>
   <si>
     <t>VT187-2697 - message box on minimize and restore application</t>
-  </si>
-  <si>
-    <t>VT187-0660 - Preload with NPAPI plugin PreloadLegacyGeneric</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=PB and RE2.2 Semi Auto Frame Work : SignatureCapture
-};
-validate2
-{
-validate_isIconDisplayed=signatureArea_xpath,true
-};</t>
-  </si>
-  <si>
-    <t>VT187-0661 - Do not Preload with NPAPI plugin PreloadLegacyGeneric</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=PB and RE2.2 Semi Auto Frame Work : SignatureCapture
-};
-validate2
-{
-validate_isIconDisplayed=signatureArea_xpath,false
-};</t>
-  </si>
-  <si>
-    <t>VT187-0670 - Preload with NPAPI plugin PreloadJSObjects</t>
-  </si>
-  <si>
-    <t>VT187-0671 - Do not Preload with NPAPI plugin PreloadJSObjects</t>
   </si>
   <si>
     <t>validate1
@@ -888,19 +853,6 @@
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
 ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="30000"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(6);
-validate1;
-link_Click(NavTimeOut_link);
-wait(35);
-validate2;
-wait(4);
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
-ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="-100"/&gt;);
 PushConfigxml;</t>
   </si>
   <si>
@@ -1410,56 +1362,14 @@
     <t>wait(6);
 validate1;
 link_Click(NavTimeOut_link);
-wait(60);
+wait(35);
 validate2;
+wait(4);
 PushBkpConfigxml;
 PullConfigxml;
 ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/All_index.html" name="Menu"/&gt;);
 ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
 PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-wait(5);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-wait(5);
-validate2;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadJSObjects, &lt;PreloadJSObjects value="1"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9100/app/Signature/index.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-wait(5);
-validate2;
-PushBkpConfigxml;
-PullConfigxml;
-ChangeConfigxml(Applications/Application/NPAPI/Preloads,PreloadLegacyGeneric, &lt;PreloadLegacyGeneric value="0"/&gt;);
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82:9098/app/SignatureCapture/generic_obj.html" name="Menu"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>wait(4);
-validate1;
-ClickRunTest(runtest_top_xpath);
-wait(5);
-validate2;
-PushBkpConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1614,7 +1524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1644,15 +1554,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1949,10 +1850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD59"/>
+  <dimension ref="A1:XFD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2025,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
@@ -2054,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>54</v>
@@ -2083,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>55</v>
@@ -39647,10 +39548,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -39676,10 +39577,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -39705,7 +39606,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>62</v>
@@ -39734,7 +39635,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>56</v>
@@ -39763,7 +39664,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>57</v>
@@ -39792,7 +39693,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>58</v>
@@ -39821,10 +39722,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -39850,10 +39751,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -39879,10 +39780,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -39908,10 +39809,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -39937,10 +39838,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -39966,10 +39867,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -39995,10 +39896,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -40024,10 +39925,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -40053,10 +39954,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -40082,10 +39983,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -40111,10 +40012,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -40140,10 +40041,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -40169,10 +40070,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -40198,10 +40099,10 @@
         <v>1</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -40227,10 +40128,10 @@
         <v>1</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -40256,7 +40157,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>61</v>
@@ -40285,10 +40186,10 @@
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -40314,10 +40215,10 @@
         <v>1</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -40343,7 +40244,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>42</v>
@@ -40372,10 +40273,10 @@
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -40401,10 +40302,10 @@
         <v>1</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -40430,7 +40331,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>59</v>
@@ -40459,10 +40360,10 @@
         <v>1</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -40488,7 +40389,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>47</v>
@@ -40517,7 +40418,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>47</v>
@@ -40526,9 +40427,9 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="141" thickBot="1">
+    <row r="36" spans="1:11" ht="166.5" thickBot="1">
       <c r="A36" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -40540,13 +40441,13 @@
         <v>10</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>47</v>
@@ -40555,9 +40456,9 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="166.5" thickBot="1">
+    <row r="37" spans="1:11" ht="179.25" thickBot="1">
       <c r="A37" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -40569,24 +40470,24 @@
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="179.25" thickBot="1">
+    <row r="38" spans="1:11" ht="153.75" thickBot="1">
       <c r="A38" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -40598,16 +40499,16 @@
         <v>10</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>132</v>
+        <v>67</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -40615,7 +40516,7 @@
     </row>
     <row r="39" spans="1:11" ht="153.75" thickBot="1">
       <c r="A39" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -40627,24 +40528,24 @@
         <v>10</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F39" s="1">
         <v>1</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="153.75" thickBot="1">
+    <row r="40" spans="1:11" ht="166.5" thickBot="1">
       <c r="A40" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -40656,24 +40557,24 @@
         <v>10</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F40" s="1">
         <v>1</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="166.5" thickBot="1">
+    <row r="41" spans="1:11" ht="294" thickBot="1">
       <c r="A41" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -40685,16 +40586,16 @@
         <v>10</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -40702,7 +40603,7 @@
     </row>
     <row r="42" spans="1:11" ht="294" thickBot="1">
       <c r="A42" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -40714,24 +40615,24 @@
         <v>10</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F42" s="1">
         <v>1</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="294" thickBot="1">
+    <row r="43" spans="1:11" ht="281.25" thickBot="1">
       <c r="A43" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -40743,16 +40644,16 @@
         <v>10</v>
       </c>
       <c r="E43" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="F43" s="1">
-        <v>1</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -40760,7 +40661,7 @@
     </row>
     <row r="44" spans="1:11" ht="281.25" thickBot="1">
       <c r="A44" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -40778,10 +40679,10 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -40789,7 +40690,7 @@
     </row>
     <row r="45" spans="1:11" ht="281.25" thickBot="1">
       <c r="A45" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -40807,10 +40708,10 @@
         <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -40818,7 +40719,7 @@
     </row>
     <row r="46" spans="1:11" ht="281.25" thickBot="1">
       <c r="A46" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -40836,18 +40737,18 @@
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="281.25" thickBot="1">
+    <row r="47" spans="1:11" ht="217.5" thickBot="1">
       <c r="A47" s="1">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -40865,18 +40766,18 @@
         <v>1</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="217.5" thickBot="1">
+    <row r="48" spans="1:11" ht="319.5" thickBot="1">
       <c r="A48" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -40894,18 +40795,18 @@
         <v>1</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="319.5" thickBot="1">
+    <row r="49" spans="1:11" ht="294" thickBot="1">
       <c r="A49" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -40923,18 +40824,18 @@
         <v>1</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="294" thickBot="1">
+    <row r="50" spans="1:11" ht="255.75" thickBot="1">
       <c r="A50" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -40952,18 +40853,18 @@
         <v>1</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="255.75" thickBot="1">
+    <row r="51" spans="1:11" ht="294" thickBot="1">
       <c r="A51" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -40981,10 +40882,10 @@
         <v>1</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -40992,7 +40893,7 @@
     </row>
     <row r="52" spans="1:11" ht="294" thickBot="1">
       <c r="A52" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
@@ -41010,18 +40911,15 @@
         <v>1</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
+        <v>71</v>
+      </c>
     </row>
-    <row r="53" spans="1:11" ht="294" thickBot="1">
+    <row r="53" spans="1:11" ht="281.25" thickBot="1">
       <c r="A53" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -41039,15 +40937,15 @@
         <v>1</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="281.25" thickBot="1">
+    <row r="54" spans="1:11" ht="294" thickBot="1">
       <c r="A54" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -41065,140 +40963,10 @@
         <v>1</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="294" thickBot="1">
-      <c r="A55" s="1">
-        <v>55</v>
-      </c>
-      <c r="B55" s="1">
-        <v>1</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F55" s="1">
-        <v>1</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="153.75" thickBot="1">
-      <c r="A56" s="1">
-        <v>56</v>
-      </c>
-      <c r="B56" s="1">
-        <v>1</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F56" s="1">
-        <v>1</v>
-      </c>
-      <c r="G56" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="H56" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="141" thickBot="1">
-      <c r="A57" s="1">
-        <v>57</v>
-      </c>
-      <c r="B57" s="11">
-        <v>1</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F57" s="1">
-        <v>1</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="H57" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="153.75" thickBot="1">
-      <c r="A58" s="1">
-        <v>58</v>
-      </c>
-      <c r="B58" s="1">
-        <v>1</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F58" s="1">
-        <v>1</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="115.5" thickBot="1">
-      <c r="A59" s="1">
-        <v>59</v>
-      </c>
-      <c r="B59" s="11">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F59" s="1">
-        <v>1</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="H59" s="13" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added testcases in config DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_Configxml_JS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7358" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7533" uniqueCount="251">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -1371,6 +1371,950 @@
 ChangeConfigxml(Configuration/Navigation,NavTimeout, &lt;NavTimeout value="45000"/&gt;);
 PushConfigxml;</t>
   </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>Logger with Log info disabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogInfo,&lt;LogInfo value="1"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileNotContains=I
+};</t>
+  </si>
+  <si>
+    <t>Logger with Log info enabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogWarning,&lt;LogWarning value="0"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogInfo,&lt;LogInfo value="0"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileContains=I
+};</t>
+  </si>
+  <si>
+    <t>Logger with Log Warning disabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogWarning,&lt;LogWarning value="1"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileNotContains=W
+};</t>
+  </si>
+  <si>
+    <t>Logger with Log Warning enabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogError,&lt;LogError value="0"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogWarning,&lt;LogWarning value="0"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteLogtxt;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileContains=W
+};</t>
+  </si>
+  <si>
+    <t>Logger with Log Error disabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogError,&lt;LogError value="1"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileNotContains=E
+};</t>
+  </si>
+  <si>
+    <t>Logger with Log Error Enabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogError,&lt;LogError value="1"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogWarning,&lt;LogWarning value="1"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogInfo,&lt;LogInfo value="1"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileContains=E
+};</t>
+  </si>
+  <si>
+    <t>Logger with LogError, LogWarning, LogInfo and LogUser Enabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogError,&lt;LogError value="0"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogWarning,&lt;LogWarning value="0"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogInfo,&lt;LogInfo value="0"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileContains=E
+validate_LogFileContains=W
+validate_LogFileContains=I
+};</t>
+  </si>
+  <si>
+    <t>Logger with LogError, LogWarning, LogInfo and LogUser Disabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+pullLogtxt;
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogError,&lt;LogError value="1"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogWarning,&lt;LogWarning value="1"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogInfo,&lt;LogInfo value="1"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogURI,&lt;LogURI value="\\sdcard\\Android\\data\\com.symbol.enterprisebrowser\\APD\\Log.txt"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_LogFileNotContains=E
+validate_LogFileNotContains=W
+validate_LogFileNotContains=I
+};</t>
+  </si>
+  <si>
+    <t>Logger with File protocol</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogURI,&lt;LogURI value="file://%INSTALLDIR%/Log.txt"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/APD/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/APD/Log.txt_pos);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_FileExists=/sdcard/Android/data/com.symbol.enterprisebrowser/APD/Log.txt
+};</t>
+  </si>
+  <si>
+    <t>Logger Path using Substitution Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogURI,&lt;LogURI value="\\sdcard\\Android\\data\\com.symbol.enterprisebrowser\Log.txt"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt_pos);
+</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_FileExists=/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt
+};</t>
+  </si>
+  <si>
+    <t>Logger with File protocol with invalid path</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogURI,&lt;LogURI value="file://%INSTALLDIR%/"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_FileNotExists=/sdcard/Android/data/com.symbol.enterprisebrowser/Log.txt
+};</t>
+  </si>
+  <si>
+    <t>File name missing inLogURI XML Tag</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Logger,LogURI,&lt;LogURI value=""/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>LogURI XML Tag  with null</t>
+  </si>
+  <si>
+    <t>wait(3);
+link_Click(keycapture_test_link);
+SelectTestToRun(VT289_011_string);
+ClickRunTest(runtest_top_xpath);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\myWeb\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>WebServer Enabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://localhost:8082/index.html);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=RE 2.2 Tests
+};</t>
+  </si>
+  <si>
+    <t>Navigate to webserver without mentioning html page</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://localhost:8082);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="1000"/&gt;endl  &lt;WebFolder VALUE="\\myWeb\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>WEBSPORT with other than 80</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://localhost:8082/index.html);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="0"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\myWeb\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>WebServer Disabled</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://localhost:8082/index.html);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>All XML tag with 'VALUE' in caps</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://www.google.com);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;
+wait(2);
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(QuitButton_xpath);
+wait(3);
+validate3;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DeviceKeys,FunctionKeysCapturable,&lt;FunctionKeysCapturable VALUE="0"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=Google
+};
+validate3
+{
+validate_AppMinimized=homescreen
+};</t>
+  </si>
+  <si>
+    <t>FunctionKeysCapturable with value 0  and ENABLEFUNCTIONKEY_Fx with value 1</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(keycapture_test_link);
+validate2;
+SelectTestToRun(VT289_024_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+sendKeyEvents(F1);
+validate4;
+sendKeyEvents(F2);
+validate5;
+sendKeyEvents(F3);
+validate6;
+sendKeyEvents(F4);
+validate7;
+sendKeyEvents(F5);
+validate8;
+sendKeyEvents(F6);
+validate9;
+sendKeyEvents(F7);
+validatea;
+sendKeyEvents(F8);
+validateb;
+sendKeyEvents(F9);
+validatec;
+sendKeyEvents(F10);
+validated;
+sendKeyEvents(F11);
+validatee;
+sendKeyEvents(F12);
+validatef;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/DeviceKeys,FunctionKeysCapturable,&lt;FunctionKeysCapturable VALUE="1"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=KeyCapture JS Test
+};
+validate3
+{
+validate_OldText_Exists=VT289-024
+};
+validate4
+{
+validate_keyCaptured=null
+};
+validate5
+{
+validate_keyCaptured=null
+};
+validate6
+{
+validate_keyCaptured=null
+};
+validate7
+{
+validate_keyCaptured=null
+};
+validate8
+{
+validate_keyCaptured=null
+};
+validate9
+{
+validate_keyCaptured=null
+};
+validatea
+{
+validate_keyCaptured=null
+};
+validateb
+{
+validate_keyCaptured=null
+};
+validatec
+{
+validate_keyCaptured=null
+};
+validated
+{
+validate_keyCaptured=null
+};
+validatee
+{
+validate_keyCaptured=null
+};
+validatef
+{
+validate_keyCaptured=null
+};</t>
+  </si>
+  <si>
+    <t>FunctionKeysCapturable with value 1 and ENABLEFUNCTIONKEY_Fx with value 1</t>
+  </si>
+  <si>
+    <t>wait(5);
+validate1;
+link_Click(keycapture_test_link);
+validate2;
+SelectTestToRun(VT289_024_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+sendKeyEvents(F1);
+validate4;
+sendKeyEvents(F2);
+validate5;
+sendKeyEvents(F3);
+validate6;
+sendKeyEvents(F4);
+validate7;
+sendKeyEvents(F5);
+validate8;
+sendKeyEvents(F6);
+validate9;
+sendKeyEvents(F7);
+validatea;
+sendKeyEvents(F8);
+validateb;
+sendKeyEvents(F9);
+validatec;
+sendKeyEvents(F10);
+validated;
+sendKeyEvents(F11);
+validatee;
+sendKeyEvents(F12);
+validatef;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application,HTTP_Proxy,&lt;HTTP_Proxy value="http://wwwgate0.mot.com:1080"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://www.google.com/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=KeyCapture JS Test
+};
+validate3
+{
+validate_OldText_Exists=VT289-024
+};
+validate4
+{
+validate_keyCaptured=131
+};
+validate5
+{
+validate_keyCaptured=132
+};
+validate6
+{
+validate_keyCaptured=133
+};
+validate7
+{
+validate_keyCaptured=134
+};
+validate8
+{
+validate_keyCaptured=135
+};
+validate9
+{
+validate_keyCaptured=136
+};
+validatea
+{
+validate_keyCaptured=137
+};
+validateb
+{
+validate_keyCaptured=138
+};
+validatec
+{
+validate_keyCaptured=139
+};
+validated
+{
+validate_keyCaptured=140
+};
+validatee
+{
+validate_keyCaptured=141
+};
+validatef
+{
+validate_keyCaptured=142
+};</t>
+  </si>
+  <si>
+    <t>Config(Browser)</t>
+  </si>
+  <si>
+    <t>Don't provide No_Proxy tag</t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,https://www.gmail.com);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Google
+};
+validate2
+{
+validate_PageTitle=Gmail
+};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP_Proxy with URL and port </t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application,HTTP_Proxy,&lt;HTTP_Proxy VALUE=""/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://www.google.com/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>HTTP_Proxy with blank</t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application,HTTPS_Proxy,&lt;HTTPS_Proxy value="http://wwwgate0.mot.com:1080"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="https://www.gmail.com/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTPS_Proxy with URL and port </t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application,HTTPS_Proxy,&lt;HTTPS_Proxy value=""/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="https://www.gmail.com/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Gmail
+};</t>
+  </si>
+  <si>
+    <t>HTTPS_Proxy with blank</t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>cookie.db file name in config</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://www.google.com);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;
+validate3;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=Google
+};
+validate3
+{
+validate_FileExists=/sdcard/Android/data/com.symbol.enterprisebrowser/cookies.db
+};</t>
+  </si>
+  <si>
+    <t>cookie.db with quit of RE</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+validate2;
+rebootDevice;
+wait(30);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_FileExists=/sdcard/Android/data/com.symbol.enterprisebrowser/cookies.db
+};</t>
+  </si>
+  <si>
+    <t>cookie.db with relaunch of RE after boot</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/Navigation,NetworkCookieDatabase,&lt;NetworkCookieDatabase value="\\sdcard\\Application\\MyCookies.db"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>cookie.db with path to application folder and name as Mycookies.db</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://10.233.85.82/neon/all_index.html" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,NetworkCookieDatabase,&lt;NetworkCookieDatabase value=""/&gt;);
+ChangeConfigxml(Configuration/DebugButtons,DebugButtonsEnabled,&lt;DebugButtonsEnabled VALUE="1"/&gt;);
+PushConfigxml;
+deleteFile(/sdcard/Application/Mycookies.db);
+deleteFile(/sdcard/Android/data/com.symbol.enterprisebrowser/cookies.db);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_FileExists=/sdcard/Application/Mycookies.db
+};</t>
+  </si>
+  <si>
+    <t>don't mention any path and name of db for NetworkCookieDatabase tag in config</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+validate2;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_FileNotExists=/sdcard/Android/data/com.symbol.enterprisebrowser/cookies.db
+validate_FileNotExists=/sdcard/Application/Mycookies.db
+};</t>
+  </si>
+  <si>
+    <t>Navigation/ UserAgent with default setting</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+TypeinAddressbar(Addressbar_xpath,http://www.google.com);
+sendKeyEvents(ENTER);
+wait(10);
+SwitchApp(WEBVIEW);
+validate2;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="https://10.233.85.82:8082/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,VerifyPeerCertificate,&lt;VerifyPeerCertificate value="0"/&gt;);
+ChangeConfigxml(Configuration/Navigation,NavTimeout,&lt;NavTimeout value="100000"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=All Index
+};
+validate2
+{
+validate_PageTitle=Google
+};</t>
+  </si>
+  <si>
+    <t>VerifyPeerCertificate 0 and browse ssl sites</t>
+  </si>
+  <si>
+    <t>wait(100);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="https://www.gmail.com/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,VerifyPeerCertificate,&lt;VerifyPeerCertificate value="0"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Javascript Application loaded from local server
+};</t>
+  </si>
+  <si>
+    <t>VerifyPeerCertificate 0 and browse non ssl sites</t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="https://10.233.85.82:8082/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,VerifyPeerCertificate,&lt;VerifyPeerCertificate value="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>VerifyPeerCertificate 1 and browse ssl sites</t>
+  </si>
+  <si>
+    <t>wait(10);
+TakeScreenshot(VT206_0377);
+validate1;
+PushBkpConfigxml;
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="https://www.gmail.com/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration/Applications/Application/Navigation,VerifyPeerCertificate,&lt;VerifyPeerCertificate value="1"/&gt;);
+PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_Screenshot=VT206_0377
+};</t>
+  </si>
+  <si>
+    <t>VerifyPeerCertificate 1 and browse non ssl sites</t>
+  </si>
+  <si>
+    <t>wait(10);
+validate1;</t>
+  </si>
 </sst>
 </file>
 
@@ -1424,7 +2368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1520,11 +2464,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1554,6 +2522,22 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1850,10 +2834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD54"/>
+  <dimension ref="A1:XFD89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39704,7 +40688,7 @@
     </row>
     <row r="11" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -39733,7 +40717,7 @@
     </row>
     <row r="12" spans="1:16384" ht="115.5" thickBot="1">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -39762,7 +40746,7 @@
     </row>
     <row r="13" spans="1:16384" ht="166.5" thickBot="1">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -39791,7 +40775,7 @@
     </row>
     <row r="14" spans="1:16384" ht="153.75" thickBot="1">
       <c r="A14" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -39820,7 +40804,7 @@
     </row>
     <row r="15" spans="1:16384" ht="192" thickBot="1">
       <c r="A15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -39849,7 +40833,7 @@
     </row>
     <row r="16" spans="1:16384" ht="192" thickBot="1">
       <c r="A16" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -39878,7 +40862,7 @@
     </row>
     <row r="17" spans="1:11" ht="204.75" thickBot="1">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -39907,7 +40891,7 @@
     </row>
     <row r="18" spans="1:11" ht="204.75" thickBot="1">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -39936,7 +40920,7 @@
     </row>
     <row r="19" spans="1:11" ht="179.25" thickBot="1">
       <c r="A19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -39965,7 +40949,7 @@
     </row>
     <row r="20" spans="1:11" ht="128.25" thickBot="1">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -39994,7 +40978,7 @@
     </row>
     <row r="21" spans="1:11" ht="166.5" thickBot="1">
       <c r="A21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -40023,7 +41007,7 @@
     </row>
     <row r="22" spans="1:11" ht="217.5" thickBot="1">
       <c r="A22" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -40052,7 +41036,7 @@
     </row>
     <row r="23" spans="1:11" ht="230.25" thickBot="1">
       <c r="A23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -40081,7 +41065,7 @@
     </row>
     <row r="24" spans="1:11" ht="230.25" thickBot="1">
       <c r="A24" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -40110,7 +41094,7 @@
     </row>
     <row r="25" spans="1:11" ht="243" thickBot="1">
       <c r="A25" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -40139,7 +41123,7 @@
     </row>
     <row r="26" spans="1:11" ht="192" thickBot="1">
       <c r="A26" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -40168,7 +41152,7 @@
     </row>
     <row r="27" spans="1:11" ht="204.75" thickBot="1">
       <c r="A27" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -40197,7 +41181,7 @@
     </row>
     <row r="28" spans="1:11" ht="179.25" thickBot="1">
       <c r="A28" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -40226,7 +41210,7 @@
     </row>
     <row r="29" spans="1:11" ht="179.25" thickBot="1">
       <c r="A29" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -40255,7 +41239,7 @@
     </row>
     <row r="30" spans="1:11" ht="192" thickBot="1">
       <c r="A30" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -40284,7 +41268,7 @@
     </row>
     <row r="31" spans="1:11" ht="179.25" thickBot="1">
       <c r="A31" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
@@ -40313,7 +41297,7 @@
     </row>
     <row r="32" spans="1:11" ht="179.25" thickBot="1">
       <c r="A32" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -40342,7 +41326,7 @@
     </row>
     <row r="33" spans="1:11" ht="153.75" thickBot="1">
       <c r="A33" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -40371,7 +41355,7 @@
     </row>
     <row r="34" spans="1:11" ht="141" thickBot="1">
       <c r="A34" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -40400,7 +41384,7 @@
     </row>
     <row r="35" spans="1:11" ht="153.75" thickBot="1">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
@@ -40429,7 +41413,7 @@
     </row>
     <row r="36" spans="1:11" ht="166.5" thickBot="1">
       <c r="A36" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -40458,7 +41442,7 @@
     </row>
     <row r="37" spans="1:11" ht="179.25" thickBot="1">
       <c r="A37" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -40487,7 +41471,7 @@
     </row>
     <row r="38" spans="1:11" ht="153.75" thickBot="1">
       <c r="A38" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -40516,7 +41500,7 @@
     </row>
     <row r="39" spans="1:11" ht="153.75" thickBot="1">
       <c r="A39" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -40545,7 +41529,7 @@
     </row>
     <row r="40" spans="1:11" ht="166.5" thickBot="1">
       <c r="A40" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -40574,7 +41558,7 @@
     </row>
     <row r="41" spans="1:11" ht="294" thickBot="1">
       <c r="A41" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -40603,7 +41587,7 @@
     </row>
     <row r="42" spans="1:11" ht="294" thickBot="1">
       <c r="A42" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -40632,7 +41616,7 @@
     </row>
     <row r="43" spans="1:11" ht="281.25" thickBot="1">
       <c r="A43" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -40661,7 +41645,7 @@
     </row>
     <row r="44" spans="1:11" ht="281.25" thickBot="1">
       <c r="A44" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -40690,7 +41674,7 @@
     </row>
     <row r="45" spans="1:11" ht="281.25" thickBot="1">
       <c r="A45" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -40719,7 +41703,7 @@
     </row>
     <row r="46" spans="1:11" ht="281.25" thickBot="1">
       <c r="A46" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -40748,7 +41732,7 @@
     </row>
     <row r="47" spans="1:11" ht="217.5" thickBot="1">
       <c r="A47" s="1">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -40777,7 +41761,7 @@
     </row>
     <row r="48" spans="1:11" ht="319.5" thickBot="1">
       <c r="A48" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -40806,7 +41790,7 @@
     </row>
     <row r="49" spans="1:11" ht="294" thickBot="1">
       <c r="A49" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -40835,7 +41819,7 @@
     </row>
     <row r="50" spans="1:11" ht="255.75" thickBot="1">
       <c r="A50" s="1">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -40864,7 +41848,7 @@
     </row>
     <row r="51" spans="1:11" ht="294" thickBot="1">
       <c r="A51" s="1">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -40893,7 +41877,7 @@
     </row>
     <row r="52" spans="1:11" ht="294" thickBot="1">
       <c r="A52" s="1">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
@@ -40919,7 +41903,7 @@
     </row>
     <row r="53" spans="1:11" ht="281.25" thickBot="1">
       <c r="A53" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -40945,7 +41929,7 @@
     </row>
     <row r="54" spans="1:11" ht="294" thickBot="1">
       <c r="A54" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -40968,6 +41952,970 @@
       <c r="H54" s="7" t="s">
         <v>111</v>
       </c>
+    </row>
+    <row r="55" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13"/>
+    </row>
+    <row r="56" spans="1:11" ht="243" thickBot="1">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+    </row>
+    <row r="57" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="13"/>
+    </row>
+    <row r="58" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="13"/>
+    </row>
+    <row r="59" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="13"/>
+    </row>
+    <row r="60" spans="1:11" ht="255.75" thickBot="1">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="13"/>
+    </row>
+    <row r="61" spans="1:11" ht="255.75" thickBot="1">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="13"/>
+    </row>
+    <row r="62" spans="1:11" ht="281.25" thickBot="1">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="13"/>
+    </row>
+    <row r="63" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+    </row>
+    <row r="64" spans="1:11" ht="243" thickBot="1">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="13"/>
+    </row>
+    <row r="65" spans="1:11" ht="166.5" thickBot="1">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="13"/>
+    </row>
+    <row r="66" spans="1:11" ht="192" thickBot="1">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H66" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="13"/>
+    </row>
+    <row r="67" spans="1:11" ht="217.5" thickBot="1">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+    </row>
+    <row r="68" spans="1:11" ht="102.75" thickBot="1">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+    </row>
+    <row r="69" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+    </row>
+    <row r="70" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="13"/>
+    </row>
+    <row r="71" spans="1:11" ht="230.25" thickBot="1">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="13"/>
+    </row>
+    <row r="72" spans="1:11" ht="281.25" thickBot="1">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="H72" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="13"/>
+    </row>
+    <row r="73" spans="1:11" ht="409.6" thickBot="1">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="H73" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="13"/>
+    </row>
+    <row r="74" spans="1:11" ht="409.6" thickBot="1">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G74" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="H74" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="13"/>
+    </row>
+    <row r="75" spans="1:11" ht="102.75" thickBot="1">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="H75" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="13"/>
+    </row>
+    <row r="76" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="H76" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="13"/>
+    </row>
+    <row r="77" spans="1:11" ht="141" thickBot="1">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="H77" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+    </row>
+    <row r="78" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="H78" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+    </row>
+    <row r="79" spans="1:11" ht="115.5" thickBot="1">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H79" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="13"/>
+    </row>
+    <row r="80" spans="1:11" ht="166.5" thickBot="1">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F80" s="1">
+        <v>1</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="H80" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="13"/>
+    </row>
+    <row r="81" spans="1:11" ht="115.5" thickBot="1">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+    </row>
+    <row r="82" spans="1:11" ht="153.75" thickBot="1">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F82" s="1">
+        <v>1</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="H82" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="13"/>
+    </row>
+    <row r="83" spans="1:11" ht="179.25" thickBot="1">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F83" s="1">
+        <v>1</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="H83" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+    </row>
+    <row r="84" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1">
+        <v>1</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="H84" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="13"/>
+    </row>
+    <row r="85" spans="1:11" ht="204.75" thickBot="1">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="H85" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+    </row>
+    <row r="86" spans="1:11" ht="115.5" thickBot="1">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="H86" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+    </row>
+    <row r="87" spans="1:11" ht="115.5" thickBot="1">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="H87" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+    </row>
+    <row r="88" spans="1:11" ht="128.25" thickBot="1">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1">
+        <v>1</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="H88" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+    </row>
+    <row r="89" spans="1:11" ht="57.75" thickBot="1">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>